<commit_message>
write readme file, add convert png script
</commit_message>
<xml_diff>
--- a/psn/FGO.xlsx
+++ b/psn/FGO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongl2/Desktop/personal/GitHub/fgo-auto-run/psn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE81AEFF-8DF0-CC43-88F7-6488868BA2B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86501F5B-98D9-3B40-8110-A4DFE62F3EAD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="460" windowWidth="32700" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="32700" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pexel LUT" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Actual" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="131">
   <si>
     <t>KEY</t>
   </si>
@@ -396,22 +397,6 @@
   </si>
   <si>
     <t>2s</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">30s  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>加载战斗</t>
-    </r>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -519,6 +504,12 @@
   </si>
   <si>
     <t>1s, 10s在程序里设定</t>
+  </si>
+  <si>
+    <t>ZHIJIER</t>
+  </si>
+  <si>
+    <t>刷新助战</t>
   </si>
 </sst>
 </file>
@@ -706,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -852,6 +843,33 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -861,12 +879,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -895,21 +907,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1324,11 +1321,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
+      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
@@ -1345,18 +1342,18 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="8"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="59" t="s">
+      <c r="C1" s="65"/>
+      <c r="D1" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59" t="s">
+      <c r="E1" s="66"/>
+      <c r="F1" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="59"/>
+      <c r="G1" s="66"/>
       <c r="H1" s="39" t="s">
         <v>63</v>
       </c>
@@ -1407,7 +1404,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="9">
         <v>102</v>
@@ -1433,16 +1430,16 @@
       <c r="H3" s="41">
         <v>1</v>
       </c>
-      <c r="I3" s="60" t="s">
+      <c r="I3" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="67" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="9">
         <v>245</v>
@@ -1468,12 +1465,12 @@
       <c r="H4" s="41">
         <v>1</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="9">
         <v>392</v>
@@ -1499,12 +1496,12 @@
       <c r="H5" s="41">
         <v>1</v>
       </c>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="9">
         <v>585</v>
@@ -1530,12 +1527,12 @@
       <c r="H6" s="41">
         <v>1</v>
       </c>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="9">
         <v>725</v>
@@ -1561,12 +1558,12 @@
       <c r="H7" s="41">
         <v>1</v>
       </c>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8" s="9">
         <v>875</v>
@@ -1592,12 +1589,12 @@
       <c r="H8" s="41">
         <v>1</v>
       </c>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" s="9">
         <v>1063</v>
@@ -1623,12 +1620,12 @@
       <c r="H9" s="41">
         <v>1</v>
       </c>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" s="9">
         <v>1203</v>
@@ -1654,12 +1651,12 @@
       <c r="H10" s="41">
         <v>1</v>
       </c>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" s="9">
         <v>1347</v>
@@ -1685,8 +1682,8 @@
       <c r="H11" s="41">
         <v>1</v>
       </c>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="10" t="s">
@@ -1716,10 +1713,10 @@
       <c r="H12" s="42">
         <v>0</v>
       </c>
-      <c r="I12" s="62" t="s">
+      <c r="I12" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="62" t="s">
+      <c r="J12" s="69" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1751,8 +1748,8 @@
       <c r="H13" s="42">
         <v>0</v>
       </c>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="10" t="s">
@@ -1782,8 +1779,8 @@
       <c r="H14" s="42">
         <v>0</v>
       </c>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="10" t="s">
@@ -1813,8 +1810,8 @@
       <c r="H15" s="42">
         <v>0</v>
       </c>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="70"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="10" t="s">
@@ -1844,8 +1841,8 @@
       <c r="H16" s="42">
         <v>0</v>
       </c>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="11" t="s">
@@ -1875,10 +1872,10 @@
       <c r="H17" s="43">
         <v>0</v>
       </c>
-      <c r="I17" s="64" t="s">
+      <c r="I17" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="64" t="s">
+      <c r="J17" s="71" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1910,8 +1907,8 @@
       <c r="H18" s="43">
         <v>0</v>
       </c>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="11" t="s">
@@ -1941,12 +1938,12 @@
       <c r="H19" s="43">
         <v>0</v>
       </c>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B20" s="12">
         <v>1795</v>
@@ -2007,10 +2004,10 @@
       <c r="H21" s="44">
         <v>1</v>
       </c>
-      <c r="I21" s="53" t="s">
+      <c r="I21" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="53" t="s">
+      <c r="J21" s="62" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2042,12 +2039,12 @@
       <c r="H22" s="44">
         <v>1</v>
       </c>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B23" s="12">
         <v>1630</v>
@@ -2073,8 +2070,8 @@
       <c r="H23" s="44">
         <v>1</v>
       </c>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="13" t="s">
@@ -2104,10 +2101,10 @@
       <c r="H24" s="45">
         <v>0</v>
       </c>
-      <c r="I24" s="68" t="s">
+      <c r="I24" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="J24" s="68" t="s">
+      <c r="J24" s="55" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2139,8 +2136,8 @@
       <c r="H25" s="45">
         <v>0</v>
       </c>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="13" t="s">
@@ -2170,8 +2167,8 @@
       <c r="H26" s="45">
         <v>0</v>
       </c>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="14" t="s">
@@ -2236,10 +2233,10 @@
       <c r="H28" s="46">
         <v>0</v>
       </c>
-      <c r="I28" s="70" t="s">
+      <c r="I28" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="J28" s="70" t="s">
+      <c r="J28" s="60" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2271,8 +2268,8 @@
       <c r="H29" s="46">
         <v>0</v>
       </c>
-      <c r="I29" s="71"/>
-      <c r="J29" s="71"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="14" t="s">
@@ -2302,8 +2299,8 @@
       <c r="H30" s="46">
         <v>0</v>
       </c>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="61"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="14" t="s">
@@ -2333,8 +2330,8 @@
       <c r="H31" s="46">
         <v>0</v>
       </c>
-      <c r="I31" s="71"/>
-      <c r="J31" s="71"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="14" t="s">
@@ -2364,8 +2361,8 @@
       <c r="H32" s="46">
         <v>0</v>
       </c>
-      <c r="I32" s="71"/>
-      <c r="J32" s="71"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="14" t="s">
@@ -2434,7 +2431,7 @@
         <v>39</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2465,10 +2462,10 @@
       <c r="H35" s="47">
         <v>0</v>
       </c>
-      <c r="I35" s="66" t="s">
+      <c r="I35" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="J35" s="66" t="s">
+      <c r="J35" s="73" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2500,8 +2497,8 @@
       <c r="H36" s="47">
         <v>0</v>
       </c>
-      <c r="I36" s="67"/>
-      <c r="J36" s="67"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="74"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="15" t="s">
@@ -2531,8 +2528,8 @@
       <c r="H37" s="47">
         <v>0</v>
       </c>
-      <c r="I37" s="67"/>
-      <c r="J37" s="67"/>
+      <c r="I37" s="74"/>
+      <c r="J37" s="74"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="15" t="s">
@@ -2562,8 +2559,8 @@
       <c r="H38" s="47">
         <v>0</v>
       </c>
-      <c r="I38" s="67"/>
-      <c r="J38" s="67"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="74"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="15" t="s">
@@ -2593,8 +2590,8 @@
       <c r="H39" s="47">
         <v>0</v>
       </c>
-      <c r="I39" s="67"/>
-      <c r="J39" s="67"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="74"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="15" t="s">
@@ -2624,8 +2621,8 @@
       <c r="H40" s="47">
         <v>0</v>
       </c>
-      <c r="I40" s="67"/>
-      <c r="J40" s="67"/>
+      <c r="I40" s="74"/>
+      <c r="J40" s="74"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="18" t="s">
@@ -2743,11 +2740,11 @@
         <v>647</v>
       </c>
       <c r="D44" s="19">
-        <f t="shared" ref="D44:D60" si="6">B44</f>
+        <f t="shared" ref="D44:D61" si="6">B44</f>
         <v>584</v>
       </c>
       <c r="E44" s="19">
-        <f t="shared" ref="E44:E60" si="7">C44</f>
+        <f t="shared" ref="E44:E61" si="7">C44</f>
         <v>647</v>
       </c>
       <c r="F44" s="33">
@@ -2789,7 +2786,7 @@
         <v>1500</v>
       </c>
       <c r="G45" s="24">
-        <f t="shared" ref="G45:G60" si="9">F45/1000</f>
+        <f t="shared" ref="G45:G61" si="9">F45/1000</f>
         <v>1.5</v>
       </c>
       <c r="H45" s="42">
@@ -2798,7 +2795,7 @@
       <c r="I45" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="J45" s="55" t="s">
+      <c r="J45" s="64" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2833,7 +2830,7 @@
       <c r="I46" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="J46" s="56"/>
+      <c r="J46" s="58"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="19" t="s">
@@ -2866,7 +2863,7 @@
       <c r="I47" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="J47" s="57"/>
+      <c r="J47" s="59"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="49" t="s">
@@ -2963,58 +2960,56 @@
         <v>0</v>
       </c>
       <c r="I50" s="49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J50" s="49"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="53">
+        <v>1255</v>
+      </c>
+      <c r="C51" s="53">
+        <v>193</v>
+      </c>
+      <c r="D51" s="53">
+        <f t="shared" si="6"/>
+        <v>1255</v>
+      </c>
+      <c r="E51" s="53">
+        <f t="shared" si="7"/>
+        <v>193</v>
+      </c>
+      <c r="F51" s="32">
+        <v>1000</v>
+      </c>
+      <c r="G51" s="23">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H51" s="41">
+        <v>0</v>
+      </c>
+      <c r="I51" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="J51" s="54"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="49">
+      <c r="B52" s="49">
         <v>150</v>
       </c>
-      <c r="C51" s="49">
+      <c r="C52" s="49">
         <v>193</v>
       </c>
-      <c r="D51" s="49">
+      <c r="D52" s="49">
         <f t="shared" si="6"/>
         <v>150</v>
-      </c>
-      <c r="E51" s="49">
-        <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="F51" s="32">
-        <v>1000</v>
-      </c>
-      <c r="G51" s="23">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="H51" s="41">
-        <v>0</v>
-      </c>
-      <c r="I51" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="J51" s="72" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="B52" s="49">
-        <v>250</v>
-      </c>
-      <c r="C52" s="49">
-        <v>193</v>
-      </c>
-      <c r="D52" s="49">
-        <f t="shared" si="6"/>
-        <v>250</v>
       </c>
       <c r="E52" s="49">
         <f t="shared" si="7"/>
@@ -3031,23 +3026,25 @@
         <v>0</v>
       </c>
       <c r="I52" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="J52" s="56"/>
+        <v>88</v>
+      </c>
+      <c r="J52" s="57" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B53" s="49">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="C53" s="49">
         <v>193</v>
       </c>
       <c r="D53" s="49">
         <f t="shared" si="6"/>
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="E53" s="49">
         <f t="shared" si="7"/>
@@ -3064,23 +3061,23 @@
         <v>0</v>
       </c>
       <c r="I53" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="J53" s="56"/>
+        <v>89</v>
+      </c>
+      <c r="J53" s="58"/>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B54" s="49">
-        <v>450</v>
+        <v>350</v>
       </c>
       <c r="C54" s="49">
         <v>193</v>
       </c>
       <c r="D54" s="49">
         <f t="shared" si="6"/>
-        <v>450</v>
+        <v>350</v>
       </c>
       <c r="E54" s="49">
         <f t="shared" si="7"/>
@@ -3097,23 +3094,23 @@
         <v>0</v>
       </c>
       <c r="I54" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="J54" s="56"/>
+        <v>90</v>
+      </c>
+      <c r="J54" s="58"/>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B55" s="49">
-        <v>550</v>
+        <v>450</v>
       </c>
       <c r="C55" s="49">
         <v>193</v>
       </c>
       <c r="D55" s="49">
         <f t="shared" si="6"/>
-        <v>550</v>
+        <v>450</v>
       </c>
       <c r="E55" s="49">
         <f t="shared" si="7"/>
@@ -3130,23 +3127,23 @@
         <v>0</v>
       </c>
       <c r="I55" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="J55" s="56"/>
+        <v>91</v>
+      </c>
+      <c r="J55" s="58"/>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B56" s="49">
-        <v>650</v>
+        <v>550</v>
       </c>
       <c r="C56" s="49">
         <v>193</v>
       </c>
       <c r="D56" s="49">
         <f t="shared" si="6"/>
-        <v>650</v>
+        <v>550</v>
       </c>
       <c r="E56" s="49">
         <f t="shared" si="7"/>
@@ -3163,23 +3160,23 @@
         <v>0</v>
       </c>
       <c r="I56" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="J56" s="56"/>
+        <v>92</v>
+      </c>
+      <c r="J56" s="58"/>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B57" s="49">
-        <v>750</v>
+        <v>650</v>
       </c>
       <c r="C57" s="49">
         <v>193</v>
       </c>
       <c r="D57" s="49">
         <f t="shared" si="6"/>
-        <v>750</v>
+        <v>650</v>
       </c>
       <c r="E57" s="49">
         <f t="shared" si="7"/>
@@ -3196,23 +3193,23 @@
         <v>0</v>
       </c>
       <c r="I57" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="J57" s="56"/>
+        <v>93</v>
+      </c>
+      <c r="J57" s="58"/>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B58" s="49">
-        <v>850</v>
+        <v>750</v>
       </c>
       <c r="C58" s="49">
         <v>193</v>
       </c>
       <c r="D58" s="49">
         <f t="shared" si="6"/>
-        <v>850</v>
+        <v>750</v>
       </c>
       <c r="E58" s="49">
         <f t="shared" si="7"/>
@@ -3229,23 +3226,23 @@
         <v>0</v>
       </c>
       <c r="I58" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="J58" s="56"/>
+        <v>94</v>
+      </c>
+      <c r="J58" s="58"/>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B59" s="49">
-        <v>950</v>
+        <v>850</v>
       </c>
       <c r="C59" s="49">
         <v>193</v>
       </c>
       <c r="D59" s="49">
         <f t="shared" si="6"/>
-        <v>950</v>
+        <v>850</v>
       </c>
       <c r="E59" s="49">
         <f t="shared" si="7"/>
@@ -3262,130 +3259,128 @@
         <v>0</v>
       </c>
       <c r="I59" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="J59" s="57"/>
+        <v>95</v>
+      </c>
+      <c r="J59" s="58"/>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="49" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B60" s="49">
-        <v>1770</v>
+        <v>950</v>
       </c>
       <c r="C60" s="49">
-        <v>60</v>
+        <v>193</v>
       </c>
       <c r="D60" s="49">
         <f t="shared" si="6"/>
-        <v>1770</v>
+        <v>950</v>
       </c>
       <c r="E60" s="49">
         <f t="shared" si="7"/>
-        <v>60</v>
+        <v>193</v>
       </c>
       <c r="F60" s="32">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G60" s="23">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H60" s="41">
         <v>0</v>
       </c>
       <c r="I60" s="50" t="s">
-        <v>102</v>
-      </c>
-      <c r="J60" s="72" t="s">
-        <v>106</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="J60" s="59"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="49" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B61" s="49">
-        <v>680</v>
+        <v>1770</v>
       </c>
       <c r="C61" s="49">
-        <v>840</v>
+        <v>60</v>
       </c>
       <c r="D61" s="49">
-        <f t="shared" ref="D61:E66" si="13">B61</f>
-        <v>680</v>
+        <f t="shared" si="6"/>
+        <v>1770</v>
       </c>
       <c r="E61" s="49">
-        <f t="shared" si="13"/>
-        <v>840</v>
+        <f t="shared" si="7"/>
+        <v>60</v>
       </c>
       <c r="F61" s="32">
         <v>2000</v>
       </c>
       <c r="G61" s="23">
-        <f t="shared" ref="G61:G66" si="14">F61/1000</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="H61" s="41">
         <v>0</v>
       </c>
       <c r="I61" s="50" t="s">
-        <v>98</v>
-      </c>
-      <c r="J61" s="57"/>
+        <v>102</v>
+      </c>
+      <c r="J61" s="57" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="49" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B62" s="49">
-        <v>1240</v>
+        <v>680</v>
       </c>
       <c r="C62" s="49">
         <v>840</v>
       </c>
       <c r="D62" s="49">
-        <f t="shared" si="13"/>
-        <v>1240</v>
+        <f t="shared" ref="D62:E67" si="13">B62</f>
+        <v>680</v>
       </c>
       <c r="E62" s="49">
         <f t="shared" si="13"/>
         <v>840</v>
       </c>
       <c r="F62" s="32">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="G62" s="23">
-        <f t="shared" si="14"/>
-        <v>30</v>
+        <f t="shared" ref="G62:G67" si="14">F62/1000</f>
+        <v>2</v>
       </c>
       <c r="H62" s="41">
         <v>0</v>
       </c>
       <c r="I62" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="J62" s="49" t="s">
-        <v>107</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="J62" s="59"/>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="49" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B63" s="49">
-        <v>250</v>
+        <v>1240</v>
       </c>
       <c r="C63" s="49">
-        <v>1040</v>
+        <v>840</v>
       </c>
       <c r="D63" s="49">
         <f t="shared" si="13"/>
-        <v>250</v>
+        <v>1240</v>
       </c>
       <c r="E63" s="49">
         <f t="shared" si="13"/>
-        <v>1040</v>
+        <v>840</v>
       </c>
       <c r="F63" s="32">
         <v>2000</v>
@@ -3398,27 +3393,29 @@
         <v>0</v>
       </c>
       <c r="I63" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="J63" s="49"/>
+        <v>97</v>
+      </c>
+      <c r="J63" s="49" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="49" t="s">
         <v>110</v>
       </c>
       <c r="B64" s="49">
-        <v>670</v>
+        <v>250</v>
       </c>
       <c r="C64" s="49">
-        <v>475</v>
+        <v>1040</v>
       </c>
       <c r="D64" s="49">
         <f t="shared" si="13"/>
-        <v>670</v>
+        <v>250</v>
       </c>
       <c r="E64" s="49">
         <f t="shared" si="13"/>
-        <v>475</v>
+        <v>1040</v>
       </c>
       <c r="F64" s="32">
         <v>2000</v>
@@ -3431,27 +3428,27 @@
         <v>0</v>
       </c>
       <c r="I64" s="50" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="J64" s="49"/>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="49" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B65" s="49">
-        <v>1260</v>
+        <v>670</v>
       </c>
       <c r="C65" s="49">
-        <v>840</v>
+        <v>475</v>
       </c>
       <c r="D65" s="49">
         <f t="shared" si="13"/>
-        <v>1260</v>
+        <v>670</v>
       </c>
       <c r="E65" s="49">
         <f t="shared" si="13"/>
-        <v>840</v>
+        <v>475</v>
       </c>
       <c r="F65" s="32">
         <v>2000</v>
@@ -3464,25 +3461,23 @@
         <v>0</v>
       </c>
       <c r="I65" s="50" t="s">
-        <v>115</v>
-      </c>
-      <c r="J65" s="49" t="s">
-        <v>117</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="J65" s="49"/>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="49" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B66" s="49">
-        <v>660</v>
+        <v>1260</v>
       </c>
       <c r="C66" s="49">
         <v>840</v>
       </c>
       <c r="D66" s="49">
         <f t="shared" si="13"/>
-        <v>660</v>
+        <v>1260</v>
       </c>
       <c r="E66" s="49">
         <f t="shared" si="13"/>
@@ -3499,32 +3494,67 @@
         <v>0</v>
       </c>
       <c r="I66" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="J66" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="J66" s="49"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" s="49">
+        <v>660</v>
+      </c>
+      <c r="C67" s="49">
+        <v>840</v>
+      </c>
+      <c r="D67" s="49">
+        <f t="shared" si="13"/>
+        <v>660</v>
+      </c>
+      <c r="E67" s="49">
+        <f t="shared" si="13"/>
+        <v>840</v>
+      </c>
+      <c r="F67" s="32">
+        <v>2000</v>
+      </c>
+      <c r="G67" s="23">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="H67" s="41">
+        <v>0</v>
+      </c>
+      <c r="I67" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="J67" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="J51:J59"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="J28:J32"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="J45:J47"/>
+    <mergeCell ref="J3:J11"/>
+    <mergeCell ref="J12:J16"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J21:J23"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="I3:I11"/>
     <mergeCell ref="I12:I16"/>
     <mergeCell ref="I17:I19"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="J52:J60"/>
+    <mergeCell ref="J61:J62"/>
+    <mergeCell ref="J28:J32"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="J45:J47"/>
     <mergeCell ref="J35:J40"/>
-    <mergeCell ref="F1:G1"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="I35:I40"/>
     <mergeCell ref="I28:I32"/>
-    <mergeCell ref="J3:J11"/>
-    <mergeCell ref="J12:J16"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="J21:J23"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sync 0323 from win
</commit_message>
<xml_diff>
--- a/psn/FGO.xlsx
+++ b/psn/FGO.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongl2/Desktop/personal/GitHub/fgo-auto-run/psn/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\fgo-auto-run\psn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD67D22A-8E46-D54E-93F0-FF163A4D114F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="20535"/>
   </bookViews>
   <sheets>
     <sheet name="Pexel LUT" sheetId="1" r:id="rId1"/>
     <sheet name="Measured" sheetId="2" r:id="rId2"/>
     <sheet name="Actual" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -296,10 +295,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>ZHIJIE0</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>ZHIJIE1</t>
   </si>
   <si>
@@ -322,10 +317,6 @@
   </si>
   <si>
     <t>ZHIJIE8</t>
-  </si>
-  <si>
-    <t>选择助战-职介-0-全</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>选择助战-职介-1-剑</t>
@@ -353,10 +344,6 @@
   </si>
   <si>
     <t>选择助战-职介-7-狂</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>选择助战-职介-8-外</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -517,11 +504,20 @@
   <si>
     <t xml:space="preserve"> →  used in py3 script now</t>
   </si>
+  <si>
+    <t>ZHIJIE9</t>
+  </si>
+  <si>
+    <t>选择助战-职介-8-全</t>
+  </si>
+  <si>
+    <t>选择助战-职介-9-特</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
@@ -864,6 +860,48 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -882,51 +920,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -961,7 +957,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6B4FA6B-D066-4644-8083-E69566C80E15}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6B4FA6B-D066-4644-8083-E69566C80E15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1010,7 +1006,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E186714-FDDD-E74D-B31E-D615057E762A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2E186714-FDDD-E74D-B31E-D615057E762A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1335,40 +1331,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
+      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="7" customWidth="1"/>
-    <col min="2" max="5" width="10.83203125" style="7"/>
-    <col min="6" max="6" width="13.83203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.625" style="7" customWidth="1"/>
+    <col min="2" max="5" width="10.875" style="7"/>
+    <col min="6" max="6" width="13.875" style="7" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="21" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="47" customWidth="1"/>
-    <col min="9" max="9" width="31.33203125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="5"/>
+    <col min="9" max="9" width="31.375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="24.625" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="10.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" ht="15.75">
       <c r="A1" s="8"/>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="70" t="s">
+      <c r="C1" s="68"/>
+      <c r="D1" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70" t="s">
+      <c r="E1" s="69"/>
+      <c r="F1" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="70"/>
+      <c r="G1" s="69"/>
       <c r="H1" s="38" t="s">
         <v>63</v>
       </c>
@@ -1386,7 +1382,7 @@
       </c>
       <c r="P1" s="55"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" ht="15.75">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1420,12 +1416,12 @@
       <c r="L2" s="6"/>
       <c r="O2" s="52"/>
       <c r="P2" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75">
       <c r="A3" s="51" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B3" s="51">
         <v>102</v>
@@ -1451,17 +1447,17 @@
       <c r="H3" s="40">
         <v>1</v>
       </c>
-      <c r="I3" s="56" t="s">
+      <c r="I3" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="70" t="s">
         <v>52</v>
       </c>
       <c r="L3" s="52"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" ht="15.75">
       <c r="A4" s="51" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B4" s="51">
         <v>245</v>
@@ -1487,13 +1483,13 @@
       <c r="H4" s="40">
         <v>1</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
       <c r="L4" s="52"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" ht="15.75">
       <c r="A5" s="51" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B5" s="51">
         <v>392</v>
@@ -1519,13 +1515,13 @@
       <c r="H5" s="40">
         <v>1</v>
       </c>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
       <c r="L5" s="52"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" ht="15.75">
       <c r="A6" s="51" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B6" s="51">
         <v>585</v>
@@ -1551,13 +1547,13 @@
       <c r="H6" s="40">
         <v>1</v>
       </c>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
       <c r="L6" s="52"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" ht="15.75">
       <c r="A7" s="51" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B7" s="51">
         <v>725</v>
@@ -1583,13 +1579,13 @@
       <c r="H7" s="40">
         <v>1</v>
       </c>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
       <c r="L7" s="52"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" ht="15.75">
       <c r="A8" s="51" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B8" s="51">
         <v>875</v>
@@ -1615,13 +1611,13 @@
       <c r="H8" s="40">
         <v>1</v>
       </c>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
       <c r="L8" s="52"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" ht="15.75">
       <c r="A9" s="51" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B9" s="51">
         <v>1063</v>
@@ -1647,13 +1643,13 @@
       <c r="H9" s="40">
         <v>1</v>
       </c>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
       <c r="L9" s="52"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" ht="15.75">
       <c r="A10" s="51" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B10" s="51">
         <v>1203</v>
@@ -1679,13 +1675,13 @@
       <c r="H10" s="40">
         <v>1</v>
       </c>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
       <c r="L10" s="52"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" ht="15.75">
       <c r="A11" s="51" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B11" s="51">
         <v>1347</v>
@@ -1711,11 +1707,11 @@
       <c r="H11" s="40">
         <v>1</v>
       </c>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
       <c r="L11" s="52"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" ht="15.75">
       <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
@@ -1743,14 +1739,14 @@
       <c r="H12" s="41">
         <v>0</v>
       </c>
-      <c r="I12" s="58" t="s">
+      <c r="I12" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="58" t="s">
+      <c r="J12" s="72" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" ht="15.75">
       <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
@@ -1778,10 +1774,10 @@
       <c r="H13" s="41">
         <v>0</v>
       </c>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.75">
       <c r="A14" s="9" t="s">
         <v>10</v>
       </c>
@@ -1809,10 +1805,10 @@
       <c r="H14" s="41">
         <v>0</v>
       </c>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="I14" s="73"/>
+      <c r="J14" s="73"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -1840,10 +1836,10 @@
       <c r="H15" s="41">
         <v>0</v>
       </c>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75">
       <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
@@ -1871,10 +1867,10 @@
       <c r="H16" s="41">
         <v>0</v>
       </c>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="10" t="s">
         <v>13</v>
       </c>
@@ -1902,15 +1898,15 @@
       <c r="H17" s="42">
         <v>0</v>
       </c>
-      <c r="I17" s="60" t="s">
+      <c r="I17" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="60" t="s">
+      <c r="J17" s="74" t="s">
         <v>53</v>
       </c>
       <c r="L17" s="53"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="10" t="s">
         <v>14</v>
       </c>
@@ -1938,11 +1934,11 @@
       <c r="H18" s="42">
         <v>0</v>
       </c>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="75"/>
       <c r="L18" s="53"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="10" t="s">
         <v>15</v>
       </c>
@@ -1970,13 +1966,13 @@
       <c r="H19" s="42">
         <v>0</v>
       </c>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="75"/>
       <c r="L19" s="53"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B20" s="11">
         <v>1795</v>
@@ -2010,7 +2006,7 @@
       </c>
       <c r="L20" s="53"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="11" t="s">
         <v>3</v>
       </c>
@@ -2038,15 +2034,15 @@
       <c r="H21" s="43">
         <v>1</v>
       </c>
-      <c r="I21" s="62" t="s">
+      <c r="I21" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="62" t="s">
+      <c r="J21" s="60" t="s">
         <v>52</v>
       </c>
       <c r="L21" s="53"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" ht="15.75">
       <c r="A22" s="11" t="s">
         <v>4</v>
       </c>
@@ -2074,13 +2070,13 @@
       <c r="H22" s="43">
         <v>1</v>
       </c>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
       <c r="L22" s="53"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B23" s="11">
         <v>1630</v>
@@ -2106,11 +2102,11 @@
       <c r="H23" s="43">
         <v>1</v>
       </c>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
       <c r="L23" s="53"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="12" t="s">
         <v>16</v>
       </c>
@@ -2138,15 +2134,15 @@
       <c r="H24" s="44">
         <v>0</v>
       </c>
-      <c r="I24" s="67" t="s">
+      <c r="I24" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="J24" s="67" t="s">
+      <c r="J24" s="66" t="s">
         <v>53</v>
       </c>
       <c r="L24" s="53"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" ht="15.75">
       <c r="A25" s="12" t="s">
         <v>17</v>
       </c>
@@ -2174,11 +2170,11 @@
       <c r="H25" s="44">
         <v>0</v>
       </c>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
       <c r="L25" s="53"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="12" t="s">
         <v>18</v>
       </c>
@@ -2206,11 +2202,11 @@
       <c r="H26" s="44">
         <v>0</v>
       </c>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
       <c r="L26" s="53"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="13" t="s">
         <v>21</v>
       </c>
@@ -2245,7 +2241,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="13" t="s">
         <v>43</v>
       </c>
@@ -2273,15 +2269,15 @@
       <c r="H28" s="45">
         <v>0</v>
       </c>
-      <c r="I28" s="71" t="s">
+      <c r="I28" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="J28" s="71" t="s">
+      <c r="J28" s="58" t="s">
         <v>61</v>
       </c>
       <c r="L28" s="53"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" ht="15.75">
       <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
@@ -2309,11 +2305,11 @@
       <c r="H29" s="45">
         <v>0</v>
       </c>
-      <c r="I29" s="72"/>
-      <c r="J29" s="72"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
       <c r="L29" s="53"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" ht="15.75">
       <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
@@ -2341,11 +2337,11 @@
       <c r="H30" s="45">
         <v>0</v>
       </c>
-      <c r="I30" s="72"/>
-      <c r="J30" s="72"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="59"/>
       <c r="L30" s="53"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" ht="15.75">
       <c r="A31" s="13" t="s">
         <v>46</v>
       </c>
@@ -2373,11 +2369,11 @@
       <c r="H31" s="45">
         <v>0</v>
       </c>
-      <c r="I31" s="72"/>
-      <c r="J31" s="72"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="59"/>
       <c r="L31" s="53"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" ht="15.75">
       <c r="A32" s="13" t="s">
         <v>47</v>
       </c>
@@ -2405,11 +2401,11 @@
       <c r="H32" s="45">
         <v>0</v>
       </c>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="59"/>
       <c r="L32" s="53"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" ht="15.75">
       <c r="A33" s="13" t="s">
         <v>48</v>
       </c>
@@ -2445,7 +2441,7 @@
       </c>
       <c r="L33" s="53"/>
     </row>
-    <row r="34" spans="1:12" ht="20">
+    <row r="34" spans="1:12" ht="15.75">
       <c r="A34" s="14" t="s">
         <v>28</v>
       </c>
@@ -2477,11 +2473,11 @@
         <v>39</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="L34" s="53"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" ht="15.75">
       <c r="A35" s="14" t="s">
         <v>22</v>
       </c>
@@ -2509,15 +2505,15 @@
       <c r="H35" s="46">
         <v>0</v>
       </c>
-      <c r="I35" s="74" t="s">
+      <c r="I35" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="J35" s="74" t="s">
+      <c r="J35" s="64" t="s">
         <v>53</v>
       </c>
       <c r="L35" s="53"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" ht="15.75">
       <c r="A36" s="14" t="s">
         <v>23</v>
       </c>
@@ -2545,11 +2541,11 @@
       <c r="H36" s="46">
         <v>0</v>
       </c>
-      <c r="I36" s="75"/>
-      <c r="J36" s="75"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
       <c r="L36" s="53"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" ht="15.75">
       <c r="A37" s="14" t="s">
         <v>24</v>
       </c>
@@ -2577,11 +2573,11 @@
       <c r="H37" s="46">
         <v>0</v>
       </c>
-      <c r="I37" s="75"/>
-      <c r="J37" s="75"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="65"/>
       <c r="L37" s="53"/>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" ht="15.75">
       <c r="A38" s="14" t="s">
         <v>25</v>
       </c>
@@ -2609,11 +2605,11 @@
       <c r="H38" s="46">
         <v>0</v>
       </c>
-      <c r="I38" s="75"/>
-      <c r="J38" s="75"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
       <c r="L38" s="53"/>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" ht="15.75">
       <c r="A39" s="14" t="s">
         <v>26</v>
       </c>
@@ -2641,11 +2637,11 @@
       <c r="H39" s="46">
         <v>0</v>
       </c>
-      <c r="I39" s="75"/>
-      <c r="J39" s="75"/>
+      <c r="I39" s="65"/>
+      <c r="J39" s="65"/>
       <c r="L39" s="53"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" ht="15.75">
       <c r="A40" s="14" t="s">
         <v>27</v>
       </c>
@@ -2673,11 +2669,11 @@
       <c r="H40" s="46">
         <v>0</v>
       </c>
-      <c r="I40" s="75"/>
-      <c r="J40" s="75"/>
+      <c r="I40" s="65"/>
+      <c r="J40" s="65"/>
       <c r="L40" s="53"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" ht="15.75">
       <c r="A41" s="17" t="s">
         <v>30</v>
       </c>
@@ -2713,7 +2709,7 @@
       </c>
       <c r="L41" s="53"/>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" ht="15.75">
       <c r="A42" s="17" t="s">
         <v>40</v>
       </c>
@@ -2748,7 +2744,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" ht="15.75">
       <c r="A43" s="17" t="s">
         <v>64</v>
       </c>
@@ -2783,7 +2779,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" ht="15.75">
       <c r="A44" s="18" t="s">
         <v>67</v>
       </c>
@@ -2818,7 +2814,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" ht="15.75">
       <c r="A45" s="18" t="s">
         <v>68</v>
       </c>
@@ -2849,11 +2845,11 @@
       <c r="I45" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="J45" s="73" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="J45" s="62" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75">
       <c r="A46" s="18" t="s">
         <v>71</v>
       </c>
@@ -2884,9 +2880,9 @@
       <c r="I46" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="J46" s="65"/>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="J46" s="63"/>
+    </row>
+    <row r="47" spans="1:12" ht="15.75">
       <c r="A47" s="18" t="s">
         <v>72</v>
       </c>
@@ -2917,9 +2913,9 @@
       <c r="I47" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="J47" s="66"/>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="J47" s="57"/>
+    </row>
+    <row r="48" spans="1:12" ht="15.75">
       <c r="A48" s="48" t="s">
         <v>76</v>
       </c>
@@ -2952,9 +2948,9 @@
       </c>
       <c r="J48" s="48"/>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" ht="15.75">
       <c r="A49" s="48" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B49" s="48">
         <v>240</v>
@@ -2981,11 +2977,11 @@
         <v>0</v>
       </c>
       <c r="I49" s="49" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J49" s="48"/>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" ht="15.75">
       <c r="A50" s="50" t="s">
         <v>78</v>
       </c>
@@ -3014,13 +3010,13 @@
         <v>0</v>
       </c>
       <c r="I50" s="48" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J50" s="48"/>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" ht="15.75">
       <c r="A51" s="50" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B51" s="51">
         <v>1255</v>
@@ -3047,16 +3043,16 @@
         <v>0</v>
       </c>
       <c r="I51" s="51" t="s">
-        <v>129</v>
-      </c>
-      <c r="J51" s="64" t="s">
-        <v>105</v>
+        <v>126</v>
+      </c>
+      <c r="J51" s="56" t="s">
+        <v>102</v>
       </c>
       <c r="L51" s="53"/>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" ht="15.75">
       <c r="A52" s="48" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B52" s="48">
         <v>150</v>
@@ -3083,14 +3079,14 @@
         <v>0</v>
       </c>
       <c r="I52" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="J52" s="65"/>
+        <v>131</v>
+      </c>
+      <c r="J52" s="63"/>
       <c r="L52" s="53"/>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" ht="15.75">
       <c r="A53" s="48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B53" s="48">
         <v>250</v>
@@ -3117,14 +3113,14 @@
         <v>0</v>
       </c>
       <c r="I53" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="J53" s="65"/>
+        <v>87</v>
+      </c>
+      <c r="J53" s="63"/>
       <c r="L53" s="53"/>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" ht="15.75">
       <c r="A54" s="48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B54" s="48">
         <v>350</v>
@@ -3151,14 +3147,14 @@
         <v>0</v>
       </c>
       <c r="I54" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="J54" s="65"/>
+        <v>88</v>
+      </c>
+      <c r="J54" s="63"/>
       <c r="L54" s="53"/>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" ht="15.75">
       <c r="A55" s="48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B55" s="48">
         <v>450</v>
@@ -3185,14 +3181,14 @@
         <v>0</v>
       </c>
       <c r="I55" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="J55" s="65"/>
+        <v>89</v>
+      </c>
+      <c r="J55" s="63"/>
       <c r="L55" s="53"/>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" ht="15.75">
       <c r="A56" s="48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B56" s="48">
         <v>550</v>
@@ -3219,14 +3215,14 @@
         <v>0</v>
       </c>
       <c r="I56" s="49" t="s">
-        <v>92</v>
-      </c>
-      <c r="J56" s="65"/>
+        <v>90</v>
+      </c>
+      <c r="J56" s="63"/>
       <c r="L56" s="53"/>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" ht="15.75">
       <c r="A57" s="48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B57" s="48">
         <v>650</v>
@@ -3253,14 +3249,14 @@
         <v>0</v>
       </c>
       <c r="I57" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="J57" s="65"/>
+        <v>91</v>
+      </c>
+      <c r="J57" s="63"/>
       <c r="L57" s="53"/>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" ht="15.75">
       <c r="A58" s="48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B58" s="48">
         <v>750</v>
@@ -3287,14 +3283,14 @@
         <v>0</v>
       </c>
       <c r="I58" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="J58" s="65"/>
+        <v>92</v>
+      </c>
+      <c r="J58" s="63"/>
       <c r="L58" s="53"/>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" ht="15.75">
       <c r="A59" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B59" s="48">
         <v>850</v>
@@ -3321,14 +3317,14 @@
         <v>0</v>
       </c>
       <c r="I59" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="J59" s="65"/>
+        <v>93</v>
+      </c>
+      <c r="J59" s="63"/>
       <c r="L59" s="53"/>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" ht="15.75">
       <c r="A60" s="48" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="B60" s="48">
         <v>950</v>
@@ -3355,14 +3351,14 @@
         <v>0</v>
       </c>
       <c r="I60" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="J60" s="66"/>
+        <v>132</v>
+      </c>
+      <c r="J60" s="57"/>
       <c r="L60" s="53"/>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" ht="15.75">
       <c r="A61" s="48" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B61" s="48">
         <v>1770</v>
@@ -3389,15 +3385,15 @@
         <v>0</v>
       </c>
       <c r="I61" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="J61" s="64" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12">
+        <v>99</v>
+      </c>
+      <c r="J61" s="56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15.75">
       <c r="A62" s="48" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B62" s="48">
         <v>680</v>
@@ -3424,13 +3420,13 @@
         <v>0</v>
       </c>
       <c r="I62" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="J62" s="66"/>
-    </row>
-    <row r="63" spans="1:12">
+        <v>95</v>
+      </c>
+      <c r="J62" s="57"/>
+    </row>
+    <row r="63" spans="1:12" ht="15.75">
       <c r="A63" s="48" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B63" s="48">
         <v>1240</v>
@@ -3457,15 +3453,15 @@
         <v>0</v>
       </c>
       <c r="I63" s="49" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J63" s="48" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" ht="15.75">
       <c r="A64" s="48" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B64" s="48">
         <v>250</v>
@@ -3492,13 +3488,13 @@
         <v>0</v>
       </c>
       <c r="I64" s="49" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J64" s="48"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" ht="15.75">
       <c r="A65" s="48" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B65" s="48">
         <v>670</v>
@@ -3525,13 +3521,13 @@
         <v>0</v>
       </c>
       <c r="I65" s="49" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J65" s="48"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" ht="15.75">
       <c r="A66" s="48" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B66" s="48">
         <v>1260</v>
@@ -3558,15 +3554,15 @@
         <v>0</v>
       </c>
       <c r="I66" s="49" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J66" s="48" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="15.75">
       <c r="A67" s="48" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B67" s="48">
         <v>660</v>
@@ -3593,12 +3589,24 @@
         <v>0</v>
       </c>
       <c r="I67" s="49" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J67" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="J3:J11"/>
+    <mergeCell ref="J12:J16"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J51:J60"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I3:I11"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="J61:J62"/>
     <mergeCell ref="J28:J32"/>
     <mergeCell ref="I21:I23"/>
@@ -3607,18 +3615,6 @@
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="I35:I40"/>
     <mergeCell ref="I28:I32"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I3:I11"/>
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="J3:J11"/>
-    <mergeCell ref="J12:J16"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J51:J60"/>
-    <mergeCell ref="J24:J26"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3626,14 +3622,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" s="2" t="s">
@@ -3653,14 +3649,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" s="3" t="s">

</xml_diff>

<commit_message>
2020-11-26, new support and gloabl var access method
</commit_message>
<xml_diff>
--- a/psn/FGO.xlsx
+++ b/psn/FGO.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\fgo-auto-run\psn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongl2/Desktop/personal/GitHub/fgo-auto-run/psn/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5B7A1B-C964-E24A-A122-D06DED8FD9BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="20535"/>
+    <workbookView xWindow="-37680" yWindow="460" windowWidth="37680" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pexel LUT" sheetId="1" r:id="rId1"/>
     <sheet name="Measured" sheetId="2" r:id="rId2"/>
     <sheet name="Actual" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="143">
   <si>
     <t>KEY</t>
   </si>
@@ -511,17 +515,47 @@
     <t>选择助战-职介-8-全</t>
   </si>
   <si>
-    <t>选择助战-职介-9-特</t>
+    <t>PYPONT</t>
+  </si>
+  <si>
+    <t>友情点快点</t>
+  </si>
+  <si>
+    <t>ZOOM</t>
+  </si>
+  <si>
+    <t>略缩图缩放</t>
+  </si>
+  <si>
+    <t>强化第一个➕号</t>
+  </si>
+  <si>
+    <t>STRSELECT</t>
+  </si>
+  <si>
+    <t>礼装选择界面第一个</t>
+  </si>
+  <si>
+    <t>CRAFTONE</t>
+  </si>
+  <si>
+    <t>ZHIJIE0</t>
+  </si>
+  <si>
+    <t>选择助战-职介-8-特</t>
+  </si>
+  <si>
+    <t>选择助战-职介-9-MIX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -584,8 +618,16 @@
       <color rgb="FFFF0000"/>
       <name val="Songti SC Regular"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -637,6 +679,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -705,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -723,15 +771,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -766,12 +805,6 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -818,12 +851,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -842,12 +869,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -860,6 +881,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -872,12 +932,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -890,39 +944,75 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -957,7 +1047,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6B4FA6B-D066-4644-8083-E69566C80E15}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6B4FA6B-D066-4644-8083-E69566C80E15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1006,7 +1096,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2E186714-FDDD-E74D-B31E-D615057E762A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E186714-FDDD-E74D-B31E-D615057E762A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1331,47 +1421,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
+      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="17.625" style="7" customWidth="1"/>
-    <col min="2" max="5" width="10.875" style="7"/>
-    <col min="6" max="6" width="13.875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="21" customWidth="1"/>
-    <col min="8" max="8" width="9.5" style="47" customWidth="1"/>
-    <col min="9" max="9" width="31.375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="24.625" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="10.875" style="5"/>
+    <col min="1" max="1" width="17.6640625" style="7" customWidth="1"/>
+    <col min="2" max="5" width="10.83203125" style="7"/>
+    <col min="6" max="6" width="13.83203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="18" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="40" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="12" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75">
+    <row r="1" spans="1:16">
       <c r="A1" s="8"/>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="69" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="69"/>
-      <c r="H1" s="38" t="s">
+      <c r="G1" s="59"/>
+      <c r="H1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="30">
+      <c r="J1" s="25">
         <v>43543</v>
       </c>
       <c r="L1" s="6" t="s">
@@ -1380,9 +1470,9 @@
       <c r="O1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="55"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75">
+      <c r="P1" s="46"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1401,10 +1491,10 @@
       <c r="F2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="34" t="s">
         <v>62</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -1414,2200 +1504,2357 @@
         <v>58</v>
       </c>
       <c r="L2" s="6"/>
-      <c r="O2" s="52"/>
+      <c r="O2" s="43"/>
       <c r="P2" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75">
-      <c r="A3" s="51" t="s">
+    <row r="3" spans="1:16">
+      <c r="A3" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="51">
+      <c r="B3" s="26">
         <v>102</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="26">
         <v>865</v>
       </c>
-      <c r="D3" s="51">
+      <c r="D3" s="26">
         <f>B3</f>
         <v>102</v>
       </c>
-      <c r="E3" s="51">
+      <c r="E3" s="26">
         <f>C3</f>
         <v>865</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="26">
         <v>3000</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="51">
         <f>F3/1000</f>
         <v>3</v>
       </c>
-      <c r="H3" s="40">
-        <v>1</v>
-      </c>
-      <c r="I3" s="70" t="s">
+      <c r="H3" s="52">
+        <v>1</v>
+      </c>
+      <c r="I3" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="70" t="s">
+      <c r="J3" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="52"/>
-    </row>
-    <row r="4" spans="1:16" ht="15.75">
-      <c r="A4" s="51" t="s">
+      <c r="L3" s="43"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="51">
+      <c r="B4" s="26">
         <v>245</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="26">
         <v>865</v>
       </c>
-      <c r="D4" s="51">
+      <c r="D4" s="26">
         <f t="shared" ref="D4:D42" si="0">B4</f>
         <v>245</v>
       </c>
-      <c r="E4" s="51">
+      <c r="E4" s="26">
         <f t="shared" ref="E4:E42" si="1">C4</f>
         <v>865</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="26">
         <v>3000</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="51">
         <f>F4/1000</f>
         <v>3</v>
       </c>
-      <c r="H4" s="40">
-        <v>1</v>
-      </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="L4" s="52"/>
-    </row>
-    <row r="5" spans="1:16" ht="15.75">
-      <c r="A5" s="51" t="s">
+      <c r="H4" s="52">
+        <v>1</v>
+      </c>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="L4" s="43"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="51">
+      <c r="B5" s="26">
         <v>392</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="26">
         <v>865</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="26">
         <f t="shared" si="0"/>
         <v>392</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="26">
         <f t="shared" si="1"/>
         <v>865</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="26">
         <v>3000</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="51">
         <f t="shared" ref="G5:G42" si="2">F5/1000</f>
         <v>3</v>
       </c>
-      <c r="H5" s="40">
-        <v>1</v>
-      </c>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="L5" s="52"/>
-    </row>
-    <row r="6" spans="1:16" ht="15.75">
-      <c r="A6" s="51" t="s">
+      <c r="H5" s="52">
+        <v>1</v>
+      </c>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="L5" s="43"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="51">
+      <c r="B6" s="26">
         <v>585</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="26">
         <v>865</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="26">
         <f t="shared" si="0"/>
         <v>585</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="26">
         <f t="shared" si="1"/>
         <v>865</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="26">
         <v>3000</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="51">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H6" s="40">
-        <v>1</v>
-      </c>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="L6" s="52"/>
-    </row>
-    <row r="7" spans="1:16" ht="15.75">
-      <c r="A7" s="51" t="s">
+      <c r="H6" s="52">
+        <v>1</v>
+      </c>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="L6" s="43"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="26">
         <v>725</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="26">
         <v>865</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="26">
         <f t="shared" si="0"/>
         <v>725</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="26">
         <f t="shared" si="1"/>
         <v>865</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="26">
         <v>3000</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="51">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H7" s="40">
-        <v>1</v>
-      </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="L7" s="52"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.75">
-      <c r="A8" s="51" t="s">
+      <c r="H7" s="52">
+        <v>1</v>
+      </c>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="L7" s="43"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="51">
+      <c r="B8" s="26">
         <v>875</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="26">
         <v>865</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="26">
         <f t="shared" si="0"/>
         <v>875</v>
       </c>
-      <c r="E8" s="51">
+      <c r="E8" s="26">
         <f t="shared" si="1"/>
         <v>865</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="26">
         <v>3000</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="51">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H8" s="40">
-        <v>1</v>
-      </c>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="L8" s="52"/>
-    </row>
-    <row r="9" spans="1:16" ht="15.75">
-      <c r="A9" s="51" t="s">
+      <c r="H8" s="52">
+        <v>1</v>
+      </c>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="L8" s="43"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="51">
+      <c r="B9" s="26">
         <v>1063</v>
       </c>
-      <c r="C9" s="51">
+      <c r="C9" s="26">
         <v>865</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="26">
         <f t="shared" si="0"/>
         <v>1063</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="26">
         <f t="shared" si="1"/>
         <v>865</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="26">
         <v>3000</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="51">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H9" s="40">
-        <v>1</v>
-      </c>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="L9" s="52"/>
-    </row>
-    <row r="10" spans="1:16" ht="15.75">
-      <c r="A10" s="51" t="s">
+      <c r="H9" s="52">
+        <v>1</v>
+      </c>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
+      <c r="L9" s="43"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="51">
+      <c r="B10" s="26">
         <v>1203</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="26">
         <v>865</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="26">
         <f t="shared" si="0"/>
         <v>1203</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E10" s="26">
         <f t="shared" si="1"/>
         <v>865</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="26">
         <v>3000</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="51">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H10" s="40">
-        <v>1</v>
-      </c>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="L10" s="52"/>
-    </row>
-    <row r="11" spans="1:16" ht="15.75">
-      <c r="A11" s="51" t="s">
+      <c r="H10" s="52">
+        <v>1</v>
+      </c>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
+      <c r="L10" s="43"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="51">
+      <c r="B11" s="26">
         <v>1347</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="26">
         <v>865</v>
       </c>
-      <c r="D11" s="51">
+      <c r="D11" s="26">
         <f t="shared" si="0"/>
         <v>1347</v>
       </c>
-      <c r="E11" s="51">
+      <c r="E11" s="26">
         <f t="shared" si="1"/>
         <v>865</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="26">
         <v>3000</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="51">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H11" s="40">
-        <v>1</v>
-      </c>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="L11" s="52"/>
-    </row>
-    <row r="12" spans="1:16" ht="15.75">
-      <c r="A12" s="9" t="s">
+      <c r="H11" s="52">
+        <v>1</v>
+      </c>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77"/>
+      <c r="L11" s="43"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="27">
         <v>200</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="27">
         <v>800</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="27">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="27">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="27">
         <v>500</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="78">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="H12" s="41">
-        <v>0</v>
-      </c>
-      <c r="I12" s="72" t="s">
+      <c r="H12" s="79">
+        <v>0</v>
+      </c>
+      <c r="I12" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="72" t="s">
+      <c r="J12" s="80" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:16">
+      <c r="A13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="27">
         <v>580</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="27">
         <v>800</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="27">
         <f t="shared" si="0"/>
         <v>580</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="27">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="27">
         <v>500</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="78">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="H13" s="41">
-        <v>0</v>
-      </c>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-    </row>
-    <row r="14" spans="1:16" ht="15.75">
-      <c r="A14" s="9" t="s">
+      <c r="H13" s="79">
+        <v>0</v>
+      </c>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="27">
         <v>960</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="27">
         <v>800</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="27">
         <f t="shared" si="0"/>
         <v>960</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="27">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="27">
         <v>500</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="78">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="H14" s="41">
-        <v>0</v>
-      </c>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-    </row>
-    <row r="15" spans="1:16" ht="15.75">
-      <c r="A15" s="9" t="s">
+      <c r="H14" s="79">
+        <v>0</v>
+      </c>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="27">
         <v>1340</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="27">
         <v>800</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="27">
         <f t="shared" si="0"/>
         <v>1340</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="27">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="27">
         <v>500</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="78">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="H15" s="41">
-        <v>0</v>
-      </c>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-    </row>
-    <row r="16" spans="1:16" ht="15.75">
-      <c r="A16" s="9" t="s">
+      <c r="H15" s="79">
+        <v>0</v>
+      </c>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="27">
         <v>1720</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="27">
         <v>800</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="27">
         <f t="shared" si="0"/>
         <v>1720</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="27">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="27">
         <v>500</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="78">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="H16" s="41">
-        <v>0</v>
-      </c>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75">
-      <c r="A17" s="10" t="s">
+      <c r="H16" s="79">
+        <v>0</v>
+      </c>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="28">
         <v>620</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="28">
         <v>340</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="28">
         <f t="shared" si="0"/>
         <v>620</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="28">
         <f t="shared" si="1"/>
         <v>340</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="28">
         <v>1000</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="82">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H17" s="42">
-        <v>0</v>
-      </c>
-      <c r="I17" s="74" t="s">
+      <c r="H17" s="83">
+        <v>0</v>
+      </c>
+      <c r="I17" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="74" t="s">
+      <c r="J17" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="L17" s="53"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75">
-      <c r="A18" s="10" t="s">
+      <c r="L17" s="44"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="28">
         <v>960</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="28">
         <v>340</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="28">
         <f t="shared" si="0"/>
         <v>960</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="28">
         <f t="shared" si="1"/>
         <v>340</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="28">
         <v>1000</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="82">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H18" s="42">
-        <v>0</v>
-      </c>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="L18" s="53"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="10" t="s">
+      <c r="H18" s="83">
+        <v>0</v>
+      </c>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="L18" s="44"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="28">
         <v>1300</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="28">
         <v>340</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="28">
         <f t="shared" si="0"/>
         <v>1300</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="28">
         <f t="shared" si="1"/>
         <v>340</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="28">
         <v>1000</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="82">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H19" s="42">
-        <v>0</v>
-      </c>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="L19" s="53"/>
-    </row>
-    <row r="20" spans="1:12" ht="15.75">
-      <c r="A20" s="11" t="s">
+      <c r="H19" s="83">
+        <v>0</v>
+      </c>
+      <c r="I19" s="85"/>
+      <c r="J19" s="85"/>
+      <c r="L19" s="44"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="29">
         <v>1795</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="29">
         <v>480</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="29">
         <f t="shared" si="0"/>
         <v>1795</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="29">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="29">
         <v>2000</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="86">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H20" s="43">
-        <v>0</v>
-      </c>
-      <c r="I20" s="11" t="s">
+      <c r="H20" s="87">
+        <v>0</v>
+      </c>
+      <c r="I20" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="L20" s="53"/>
-    </row>
-    <row r="21" spans="1:12" ht="15.75">
-      <c r="A21" s="11" t="s">
+      <c r="L20" s="44"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="29">
         <v>1360</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="29">
         <v>465</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="29">
         <f t="shared" si="0"/>
         <v>1360</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="29">
         <f t="shared" si="1"/>
         <v>465</v>
       </c>
-      <c r="F21" s="34">
+      <c r="F21" s="29">
         <v>3000</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="86">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H21" s="43">
-        <v>1</v>
-      </c>
-      <c r="I21" s="60" t="s">
+      <c r="H21" s="87">
+        <v>1</v>
+      </c>
+      <c r="I21" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="60" t="s">
+      <c r="J21" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="L21" s="53"/>
-    </row>
-    <row r="22" spans="1:12" ht="15.75">
-      <c r="A22" s="11" t="s">
+      <c r="L21" s="44"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="29">
         <v>1495</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="29">
         <v>465</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="29">
         <f t="shared" si="0"/>
         <v>1495</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="29">
         <f t="shared" si="1"/>
         <v>465</v>
       </c>
-      <c r="F22" s="34">
+      <c r="F22" s="29">
         <v>3000</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="86">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H22" s="43">
-        <v>1</v>
-      </c>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="L22" s="53"/>
-    </row>
-    <row r="23" spans="1:12" ht="15.75">
-      <c r="A23" s="11" t="s">
+      <c r="H22" s="87">
+        <v>1</v>
+      </c>
+      <c r="I22" s="89"/>
+      <c r="J22" s="89"/>
+      <c r="L22" s="44"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="29">
         <v>1630</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="29">
         <v>465</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="29">
         <f t="shared" si="0"/>
         <v>1630</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="29">
         <f t="shared" si="1"/>
         <v>465</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="29">
         <v>3000</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="86">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H23" s="43">
-        <v>1</v>
-      </c>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="L23" s="53"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.75">
-      <c r="A24" s="12" t="s">
+      <c r="H23" s="87">
+        <v>1</v>
+      </c>
+      <c r="I23" s="89"/>
+      <c r="J23" s="89"/>
+      <c r="L23" s="44"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="9">
         <v>800</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="9">
         <v>60</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="9">
         <f t="shared" si="0"/>
         <v>800</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="9">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F24" s="35">
+      <c r="F24" s="30">
         <v>1000</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="21">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H24" s="44">
-        <v>0</v>
-      </c>
-      <c r="I24" s="66" t="s">
+      <c r="H24" s="37">
+        <v>0</v>
+      </c>
+      <c r="I24" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="J24" s="66" t="s">
+      <c r="J24" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="L24" s="53"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.75">
-      <c r="A25" s="12" t="s">
+      <c r="L24" s="44"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="9">
         <v>435</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="9">
         <v>60</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="9">
         <f t="shared" si="0"/>
         <v>435</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="9">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F25" s="35">
+      <c r="F25" s="30">
         <v>1000</v>
       </c>
-      <c r="G25" s="26">
+      <c r="G25" s="21">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H25" s="44">
-        <v>0</v>
-      </c>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-      <c r="L25" s="53"/>
-    </row>
-    <row r="26" spans="1:12" ht="15.75">
-      <c r="A26" s="12" t="s">
+      <c r="H25" s="37">
+        <v>0</v>
+      </c>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="L25" s="44"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="9">
         <v>70</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="9">
         <v>60</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="9">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="9">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F26" s="35">
+      <c r="F26" s="30">
         <v>1000</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="21">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H26" s="44">
-        <v>0</v>
-      </c>
-      <c r="I26" s="67"/>
-      <c r="J26" s="67"/>
-      <c r="L26" s="53"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.75">
-      <c r="A27" s="13" t="s">
+      <c r="H26" s="37">
+        <v>0</v>
+      </c>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="L26" s="44"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="10">
         <v>1649</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="10">
         <v>225</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="10">
         <f t="shared" si="0"/>
         <v>1649</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="10">
         <f t="shared" si="1"/>
         <v>225</v>
       </c>
-      <c r="F27" s="36">
+      <c r="F27" s="31">
         <v>1000</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="22">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H27" s="45">
-        <v>0</v>
-      </c>
-      <c r="I27" s="13" t="s">
+      <c r="H27" s="38">
+        <v>0</v>
+      </c>
+      <c r="I27" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="13" t="s">
+      <c r="J27" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
-      <c r="A28" s="13" t="s">
+    <row r="28" spans="1:12">
+      <c r="A28" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B28" s="10">
         <v>482</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="10">
         <v>720</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="10">
         <f t="shared" si="0"/>
         <v>482</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="10">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="F28" s="36">
+      <c r="F28" s="31">
         <v>5000</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="22">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H28" s="45">
-        <v>0</v>
-      </c>
-      <c r="I28" s="58" t="s">
+      <c r="H28" s="38">
+        <v>0</v>
+      </c>
+      <c r="I28" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="J28" s="58" t="s">
+      <c r="J28" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="L28" s="53"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75">
-      <c r="A29" s="13" t="s">
+      <c r="L28" s="44"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B29" s="10">
         <v>992</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="10">
         <v>720</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="10">
         <f t="shared" si="0"/>
         <v>992</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="10">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="F29" s="36">
+      <c r="F29" s="31">
         <v>5000</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G29" s="22">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H29" s="45">
-        <v>0</v>
-      </c>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
-      <c r="L29" s="53"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.75">
-      <c r="A30" s="13" t="s">
+      <c r="H29" s="38">
+        <v>0</v>
+      </c>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
+      <c r="L29" s="44"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30" s="10">
         <v>1446</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="10">
         <v>720</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="10">
         <f t="shared" si="0"/>
         <v>1446</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="10">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="F30" s="36">
+      <c r="F30" s="31">
         <v>5000</v>
       </c>
-      <c r="G30" s="27">
+      <c r="G30" s="22">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H30" s="45">
-        <v>0</v>
-      </c>
-      <c r="I30" s="59"/>
-      <c r="J30" s="59"/>
-      <c r="L30" s="53"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75">
-      <c r="A31" s="13" t="s">
+      <c r="H30" s="38">
+        <v>0</v>
+      </c>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
+      <c r="L30" s="44"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31" s="10">
         <v>737</v>
       </c>
-      <c r="C31" s="54">
+      <c r="C31" s="45">
         <v>720</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="10">
         <f t="shared" si="0"/>
         <v>737</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="10">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="F31" s="36">
+      <c r="F31" s="31">
         <v>5000</v>
       </c>
-      <c r="G31" s="27">
+      <c r="G31" s="22">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H31" s="45">
-        <v>0</v>
-      </c>
-      <c r="I31" s="59"/>
-      <c r="J31" s="59"/>
-      <c r="L31" s="53"/>
-    </row>
-    <row r="32" spans="1:12" ht="15.75">
-      <c r="A32" s="13" t="s">
+      <c r="H31" s="38">
+        <v>0</v>
+      </c>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
+      <c r="L31" s="44"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="10">
         <v>1219</v>
       </c>
-      <c r="C32" s="54">
+      <c r="C32" s="45">
         <v>720</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="10">
         <f t="shared" si="0"/>
         <v>1219</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="10">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="F32" s="36">
+      <c r="F32" s="31">
         <v>5000</v>
       </c>
-      <c r="G32" s="27">
+      <c r="G32" s="22">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H32" s="45">
-        <v>0</v>
-      </c>
-      <c r="I32" s="59"/>
-      <c r="J32" s="59"/>
-      <c r="L32" s="53"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.75">
-      <c r="A33" s="13" t="s">
+      <c r="H32" s="38">
+        <v>0</v>
+      </c>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="L32" s="44"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="10">
         <v>992</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="10">
         <v>720</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="10">
         <f t="shared" si="0"/>
         <v>992</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="10">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="F33" s="36">
+      <c r="F33" s="31">
         <v>5000</v>
       </c>
-      <c r="G33" s="27">
+      <c r="G33" s="22">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H33" s="45">
-        <v>0</v>
-      </c>
-      <c r="I33" s="19" t="s">
+      <c r="H33" s="38">
+        <v>0</v>
+      </c>
+      <c r="I33" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="J33" s="19" t="s">
+      <c r="J33" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="L33" s="53"/>
-    </row>
-    <row r="34" spans="1:12" ht="15.75">
-      <c r="A34" s="14" t="s">
+      <c r="L33" s="44"/>
+    </row>
+    <row r="34" spans="1:12" ht="20">
+      <c r="A34" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="11">
         <v>963</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="11">
         <v>936</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="11">
         <f t="shared" si="0"/>
         <v>963</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="11">
         <f t="shared" si="1"/>
         <v>936</v>
       </c>
-      <c r="F34" s="37">
+      <c r="F34" s="32">
         <v>1000</v>
       </c>
-      <c r="G34" s="28">
+      <c r="G34" s="23">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H34" s="46">
-        <v>0</v>
-      </c>
-      <c r="I34" s="20" t="s">
+      <c r="H34" s="39">
+        <v>0</v>
+      </c>
+      <c r="I34" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="J34" s="14" t="s">
+      <c r="J34" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="L34" s="53"/>
-    </row>
-    <row r="35" spans="1:12" ht="15.75">
-      <c r="A35" s="14" t="s">
+      <c r="L34" s="44"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35" s="11">
         <v>220</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="11">
         <v>520</v>
       </c>
-      <c r="D35" s="14">
+      <c r="D35" s="11">
         <f t="shared" si="0"/>
         <v>220</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="11">
         <f t="shared" si="1"/>
         <v>520</v>
       </c>
-      <c r="F35" s="37">
+      <c r="F35" s="32">
         <v>1000</v>
       </c>
-      <c r="G35" s="28">
+      <c r="G35" s="23">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H35" s="46">
-        <v>0</v>
-      </c>
-      <c r="I35" s="64" t="s">
+      <c r="H35" s="39">
+        <v>0</v>
+      </c>
+      <c r="I35" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="J35" s="64" t="s">
+      <c r="J35" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="L35" s="53"/>
-    </row>
-    <row r="36" spans="1:12" ht="15.75">
-      <c r="A36" s="14" t="s">
+      <c r="L35" s="44"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="11">
         <v>520</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="11">
         <v>520</v>
       </c>
-      <c r="D36" s="14">
+      <c r="D36" s="11">
         <f t="shared" si="0"/>
         <v>520</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="11">
         <f t="shared" si="1"/>
         <v>520</v>
       </c>
-      <c r="F36" s="37">
+      <c r="F36" s="32">
         <v>1000</v>
       </c>
-      <c r="G36" s="28">
+      <c r="G36" s="23">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H36" s="46">
-        <v>0</v>
-      </c>
-      <c r="I36" s="65"/>
-      <c r="J36" s="65"/>
-      <c r="L36" s="53"/>
-    </row>
-    <row r="37" spans="1:12" ht="15.75">
-      <c r="A37" s="14" t="s">
+      <c r="H36" s="39">
+        <v>0</v>
+      </c>
+      <c r="I36" s="67"/>
+      <c r="J36" s="67"/>
+      <c r="L36" s="44"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="11">
         <v>820</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C37" s="11">
         <v>520</v>
       </c>
-      <c r="D37" s="14">
+      <c r="D37" s="11">
         <f t="shared" si="0"/>
         <v>820</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="11">
         <f t="shared" si="1"/>
         <v>520</v>
       </c>
-      <c r="F37" s="37">
+      <c r="F37" s="32">
         <v>1000</v>
       </c>
-      <c r="G37" s="28">
+      <c r="G37" s="23">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H37" s="46">
-        <v>0</v>
-      </c>
-      <c r="I37" s="65"/>
-      <c r="J37" s="65"/>
-      <c r="L37" s="53"/>
-    </row>
-    <row r="38" spans="1:12" ht="15.75">
-      <c r="A38" s="14" t="s">
+      <c r="H37" s="39">
+        <v>0</v>
+      </c>
+      <c r="I37" s="67"/>
+      <c r="J37" s="67"/>
+      <c r="L37" s="44"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="11">
         <v>1120</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="11">
         <v>520</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="11">
         <f t="shared" si="0"/>
         <v>1120</v>
       </c>
-      <c r="E38" s="14">
+      <c r="E38" s="11">
         <f t="shared" si="1"/>
         <v>520</v>
       </c>
-      <c r="F38" s="37">
+      <c r="F38" s="32">
         <v>1000</v>
       </c>
-      <c r="G38" s="28">
+      <c r="G38" s="23">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H38" s="46">
-        <v>0</v>
-      </c>
-      <c r="I38" s="65"/>
-      <c r="J38" s="65"/>
-      <c r="L38" s="53"/>
-    </row>
-    <row r="39" spans="1:12" ht="15.75">
-      <c r="A39" s="14" t="s">
+      <c r="H38" s="39">
+        <v>0</v>
+      </c>
+      <c r="I38" s="67"/>
+      <c r="J38" s="67"/>
+      <c r="L38" s="44"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="14">
+      <c r="B39" s="11">
         <v>1420</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="11">
         <v>520</v>
       </c>
-      <c r="D39" s="14">
+      <c r="D39" s="11">
         <f t="shared" si="0"/>
         <v>1420</v>
       </c>
-      <c r="E39" s="14">
+      <c r="E39" s="11">
         <f t="shared" si="1"/>
         <v>520</v>
       </c>
-      <c r="F39" s="37">
+      <c r="F39" s="32">
         <v>1000</v>
       </c>
-      <c r="G39" s="28">
+      <c r="G39" s="23">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H39" s="46">
-        <v>0</v>
-      </c>
-      <c r="I39" s="65"/>
-      <c r="J39" s="65"/>
-      <c r="L39" s="53"/>
-    </row>
-    <row r="40" spans="1:12" ht="15.75">
-      <c r="A40" s="14" t="s">
+      <c r="H39" s="39">
+        <v>0</v>
+      </c>
+      <c r="I39" s="67"/>
+      <c r="J39" s="67"/>
+      <c r="L39" s="44"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="14">
+      <c r="B40" s="11">
         <v>1720</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="11">
         <v>520</v>
       </c>
-      <c r="D40" s="14">
+      <c r="D40" s="11">
         <f t="shared" si="0"/>
         <v>1720</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="11">
         <f t="shared" si="1"/>
         <v>520</v>
       </c>
-      <c r="F40" s="37">
+      <c r="F40" s="32">
         <v>1000</v>
       </c>
-      <c r="G40" s="28">
+      <c r="G40" s="23">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H40" s="46">
-        <v>0</v>
-      </c>
-      <c r="I40" s="65"/>
-      <c r="J40" s="65"/>
-      <c r="L40" s="53"/>
-    </row>
-    <row r="41" spans="1:12" ht="15.75">
-      <c r="A41" s="17" t="s">
+      <c r="H40" s="39">
+        <v>0</v>
+      </c>
+      <c r="I40" s="67"/>
+      <c r="J40" s="67"/>
+      <c r="L40" s="44"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="17">
+      <c r="B41" s="14">
         <v>1700</v>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="14">
         <v>900</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="14">
         <f t="shared" si="0"/>
         <v>1700</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E41" s="14">
         <f t="shared" si="1"/>
         <v>900</v>
       </c>
-      <c r="F41" s="31">
+      <c r="F41" s="26">
         <v>2000</v>
       </c>
-      <c r="G41" s="22">
+      <c r="G41" s="19">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H41" s="40">
-        <v>0</v>
-      </c>
-      <c r="I41" s="17" t="s">
+      <c r="H41" s="35">
+        <v>0</v>
+      </c>
+      <c r="I41" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="J41" s="17" t="s">
+      <c r="J41" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="L41" s="53"/>
-    </row>
-    <row r="42" spans="1:12" ht="15.75">
-      <c r="A42" s="17" t="s">
+      <c r="L41" s="44"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="17">
+      <c r="B42" s="14">
         <v>1780</v>
       </c>
-      <c r="C42" s="17">
+      <c r="C42" s="14">
         <v>1010</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="14">
         <f t="shared" si="0"/>
         <v>1780</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="14">
         <f t="shared" si="1"/>
         <v>1010</v>
       </c>
-      <c r="F42" s="31">
+      <c r="F42" s="26">
         <v>30000</v>
       </c>
-      <c r="G42" s="22">
+      <c r="G42" s="19">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H42" s="40">
-        <v>0</v>
-      </c>
-      <c r="I42" s="17" t="s">
+      <c r="H42" s="35">
+        <v>0</v>
+      </c>
+      <c r="I42" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="J42" s="17" t="s">
+      <c r="J42" s="14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75">
-      <c r="A43" s="17" t="s">
+    <row r="43" spans="1:12">
+      <c r="A43" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B43" s="14">
         <v>1660</v>
       </c>
-      <c r="C43" s="17">
+      <c r="C43" s="14">
         <v>1010</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="14">
         <f t="shared" ref="D43" si="3">B43</f>
         <v>1660</v>
       </c>
-      <c r="E43" s="17">
+      <c r="E43" s="14">
         <f t="shared" ref="E43" si="4">C43</f>
         <v>1010</v>
       </c>
-      <c r="F43" s="31">
+      <c r="F43" s="26">
         <v>1000</v>
       </c>
-      <c r="G43" s="22">
+      <c r="G43" s="19">
         <f t="shared" ref="G43" si="5">F43/1000</f>
         <v>1</v>
       </c>
-      <c r="H43" s="40">
-        <v>0</v>
-      </c>
-      <c r="I43" s="17" t="s">
+      <c r="H43" s="35">
+        <v>0</v>
+      </c>
+      <c r="I43" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="J43" s="17" t="s">
+      <c r="J43" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75">
-      <c r="A44" s="18" t="s">
+    <row r="44" spans="1:12">
+      <c r="A44" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="18">
+      <c r="B44" s="15">
         <v>584</v>
       </c>
-      <c r="C44" s="18">
+      <c r="C44" s="15">
         <v>647</v>
       </c>
-      <c r="D44" s="18">
-        <f t="shared" ref="D44:D61" si="6">B44</f>
+      <c r="D44" s="15">
+        <f t="shared" ref="D44:D62" si="6">B44</f>
         <v>584</v>
       </c>
-      <c r="E44" s="18">
-        <f t="shared" ref="E44:E61" si="7">C44</f>
+      <c r="E44" s="15">
+        <f t="shared" ref="E44:E62" si="7">C44</f>
         <v>647</v>
       </c>
-      <c r="F44" s="32">
+      <c r="F44" s="27">
         <v>200</v>
       </c>
-      <c r="G44" s="23">
+      <c r="G44" s="20">
         <f t="shared" ref="G44" si="8">F44/1000</f>
         <v>0.2</v>
       </c>
-      <c r="H44" s="41">
-        <v>0</v>
-      </c>
-      <c r="I44" s="18" t="s">
+      <c r="H44" s="36">
+        <v>0</v>
+      </c>
+      <c r="I44" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="J44" s="18" t="s">
+      <c r="J44" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75">
-      <c r="A45" s="18" t="s">
+    <row r="45" spans="1:12">
+      <c r="A45" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="18">
+      <c r="B45" s="15">
         <v>1710</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="15">
         <v>365</v>
       </c>
-      <c r="D45" s="18">
+      <c r="D45" s="15">
         <f t="shared" si="6"/>
         <v>1710</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E45" s="15">
         <f t="shared" si="7"/>
         <v>365</v>
       </c>
-      <c r="F45" s="32">
+      <c r="F45" s="27">
         <v>2000</v>
       </c>
-      <c r="G45" s="23">
-        <f t="shared" ref="G45:G61" si="9">F45/1000</f>
+      <c r="G45" s="20">
+        <f t="shared" ref="G45:G62" si="9">F45/1000</f>
         <v>2</v>
       </c>
-      <c r="H45" s="41">
-        <v>0</v>
-      </c>
-      <c r="I45" s="18" t="s">
+      <c r="H45" s="36">
+        <v>0</v>
+      </c>
+      <c r="I45" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="J45" s="62" t="s">
+      <c r="J45" s="64" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75">
-      <c r="A46" s="18" t="s">
+    <row r="46" spans="1:12">
+      <c r="A46" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="18">
+      <c r="B46" s="15">
         <v>1255</v>
       </c>
-      <c r="C46" s="18">
+      <c r="C46" s="15">
         <v>840</v>
       </c>
-      <c r="D46" s="18">
+      <c r="D46" s="15">
         <f t="shared" si="6"/>
         <v>1255</v>
       </c>
-      <c r="E46" s="18">
+      <c r="E46" s="15">
         <f t="shared" si="7"/>
         <v>840</v>
       </c>
-      <c r="F46" s="32">
+      <c r="F46" s="27">
         <v>3000</v>
       </c>
-      <c r="G46" s="23">
+      <c r="G46" s="20">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="H46" s="41">
-        <v>0</v>
-      </c>
-      <c r="I46" s="18" t="s">
+      <c r="H46" s="36">
+        <v>0</v>
+      </c>
+      <c r="I46" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="J46" s="63"/>
-    </row>
-    <row r="47" spans="1:12" ht="15.75">
-      <c r="A47" s="18" t="s">
+      <c r="J46" s="65"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="18">
+      <c r="B47" s="15">
         <v>960</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C47" s="15">
         <v>840</v>
       </c>
-      <c r="D47" s="18">
+      <c r="D47" s="15">
         <f t="shared" si="6"/>
         <v>960</v>
       </c>
-      <c r="E47" s="18">
+      <c r="E47" s="15">
         <f t="shared" si="7"/>
         <v>840</v>
       </c>
-      <c r="F47" s="32">
+      <c r="F47" s="27">
         <v>2000</v>
       </c>
-      <c r="G47" s="23">
+      <c r="G47" s="20">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="H47" s="41">
-        <v>0</v>
-      </c>
-      <c r="I47" s="18" t="s">
+      <c r="H47" s="36">
+        <v>0</v>
+      </c>
+      <c r="I47" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="J47" s="57"/>
-    </row>
-    <row r="48" spans="1:12" ht="15.75">
-      <c r="A48" s="48" t="s">
+      <c r="J47" s="61"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="B48" s="48">
+      <c r="B48" s="70">
         <v>1050</v>
       </c>
-      <c r="C48" s="48">
+      <c r="C48" s="70">
         <v>345</v>
       </c>
-      <c r="D48" s="48">
+      <c r="D48" s="70">
         <f t="shared" si="6"/>
         <v>1050</v>
       </c>
-      <c r="E48" s="48">
+      <c r="E48" s="70">
         <f t="shared" si="7"/>
         <v>345</v>
       </c>
-      <c r="F48" s="31">
+      <c r="F48" s="71">
         <v>3000</v>
       </c>
-      <c r="G48" s="22">
+      <c r="G48" s="72">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="H48" s="40">
-        <v>0</v>
-      </c>
-      <c r="I48" s="49" t="s">
+      <c r="H48" s="73">
+        <v>0</v>
+      </c>
+      <c r="I48" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="J48" s="48"/>
-    </row>
-    <row r="49" spans="1:12" ht="15.75">
-      <c r="A49" s="48" t="s">
+      <c r="J48" s="70"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="48">
+      <c r="B49" s="70">
         <v>240</v>
       </c>
-      <c r="C49" s="48">
+      <c r="C49" s="70">
         <v>465</v>
       </c>
-      <c r="D49" s="48">
+      <c r="D49" s="70">
         <f t="shared" ref="D49" si="10">B49</f>
         <v>240</v>
       </c>
-      <c r="E49" s="48">
+      <c r="E49" s="70">
         <f t="shared" ref="E49" si="11">C49</f>
         <v>465</v>
       </c>
-      <c r="F49" s="31">
+      <c r="F49" s="71">
         <v>3000</v>
       </c>
-      <c r="G49" s="22">
+      <c r="G49" s="72">
         <f t="shared" ref="G49" si="12">F49/1000</f>
         <v>3</v>
       </c>
-      <c r="H49" s="40">
-        <v>0</v>
-      </c>
-      <c r="I49" s="49" t="s">
+      <c r="H49" s="73">
+        <v>0</v>
+      </c>
+      <c r="I49" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="J49" s="48"/>
-    </row>
-    <row r="50" spans="1:12" ht="15.75">
-      <c r="A50" s="50" t="s">
+      <c r="J49" s="70"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="48">
+      <c r="B50" s="70">
         <v>335</v>
       </c>
-      <c r="C50" s="48">
+      <c r="C50" s="70">
         <v>1040</v>
       </c>
-      <c r="D50" s="48">
+      <c r="D50" s="70">
         <f t="shared" si="6"/>
         <v>335</v>
       </c>
-      <c r="E50" s="48">
+      <c r="E50" s="70">
         <f t="shared" si="7"/>
         <v>1040</v>
       </c>
-      <c r="F50" s="31">
+      <c r="F50" s="71">
         <v>1000</v>
       </c>
-      <c r="G50" s="22">
+      <c r="G50" s="72">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="H50" s="40">
-        <v>0</v>
-      </c>
-      <c r="I50" s="48" t="s">
+      <c r="H50" s="73">
+        <v>0</v>
+      </c>
+      <c r="I50" s="70" t="s">
         <v>104</v>
       </c>
-      <c r="J50" s="48"/>
-    </row>
-    <row r="51" spans="1:12" ht="15.75">
-      <c r="A51" s="50" t="s">
+      <c r="J50" s="70"/>
+    </row>
+    <row r="51" spans="1:12" s="54" customFormat="1">
+      <c r="A51" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="B51" s="51">
-        <v>1255</v>
-      </c>
-      <c r="C51" s="51">
+      <c r="B51" s="26">
+        <v>1277</v>
+      </c>
+      <c r="C51" s="26">
         <v>193</v>
       </c>
-      <c r="D51" s="51">
+      <c r="D51" s="26">
         <f t="shared" si="6"/>
-        <v>1255</v>
-      </c>
-      <c r="E51" s="51">
+        <v>1277</v>
+      </c>
+      <c r="E51" s="26">
         <f t="shared" si="7"/>
         <v>193</v>
       </c>
-      <c r="F51" s="31">
+      <c r="F51" s="26">
         <v>1000</v>
       </c>
-      <c r="G51" s="22">
+      <c r="G51" s="51">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="H51" s="40">
-        <v>0</v>
-      </c>
-      <c r="I51" s="51" t="s">
+      <c r="H51" s="52">
+        <v>0</v>
+      </c>
+      <c r="I51" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="J51" s="56" t="s">
+      <c r="J51" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="L51" s="53"/>
-    </row>
-    <row r="52" spans="1:12" ht="15.75">
-      <c r="A52" s="48" t="s">
+      <c r="L51" s="55"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B52" s="26">
+        <v>140</v>
+      </c>
+      <c r="C52" s="26">
+        <v>195</v>
+      </c>
+      <c r="D52" s="26">
+        <f t="shared" si="6"/>
+        <v>140</v>
+      </c>
+      <c r="E52" s="26">
+        <f t="shared" si="7"/>
+        <v>195</v>
+      </c>
+      <c r="F52" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G52" s="51">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H52" s="52">
+        <v>0</v>
+      </c>
+      <c r="I52" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="J52" s="68"/>
+      <c r="L52" s="44"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="26">
+        <v>241</v>
+      </c>
+      <c r="C53" s="26">
+        <v>195</v>
+      </c>
+      <c r="D53" s="26">
+        <f t="shared" si="6"/>
+        <v>241</v>
+      </c>
+      <c r="E53" s="26">
+        <f t="shared" si="7"/>
+        <v>195</v>
+      </c>
+      <c r="F53" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G53" s="51">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H53" s="52">
+        <v>0</v>
+      </c>
+      <c r="I53" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="J53" s="68"/>
+      <c r="L53" s="44"/>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54" s="26">
+        <v>342</v>
+      </c>
+      <c r="C54" s="26">
+        <v>195</v>
+      </c>
+      <c r="D54" s="26">
+        <f t="shared" si="6"/>
+        <v>342</v>
+      </c>
+      <c r="E54" s="26">
+        <f t="shared" si="7"/>
+        <v>195</v>
+      </c>
+      <c r="F54" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G54" s="51">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H54" s="52">
+        <v>0</v>
+      </c>
+      <c r="I54" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="J54" s="68"/>
+      <c r="L54" s="44"/>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="26">
+        <v>443</v>
+      </c>
+      <c r="C55" s="26">
+        <v>195</v>
+      </c>
+      <c r="D55" s="26">
+        <f t="shared" si="6"/>
+        <v>443</v>
+      </c>
+      <c r="E55" s="26">
+        <f t="shared" si="7"/>
+        <v>195</v>
+      </c>
+      <c r="F55" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G55" s="51">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H55" s="52">
+        <v>0</v>
+      </c>
+      <c r="I55" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="J55" s="68"/>
+      <c r="L55" s="44"/>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" s="26">
+        <v>544</v>
+      </c>
+      <c r="C56" s="26">
+        <v>195</v>
+      </c>
+      <c r="D56" s="26">
+        <f t="shared" si="6"/>
+        <v>544</v>
+      </c>
+      <c r="E56" s="26">
+        <f t="shared" si="7"/>
+        <v>195</v>
+      </c>
+      <c r="F56" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G56" s="51">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H56" s="52">
+        <v>0</v>
+      </c>
+      <c r="I56" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="J56" s="68"/>
+      <c r="L56" s="44"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B57" s="26">
+        <v>645</v>
+      </c>
+      <c r="C57" s="26">
+        <v>195</v>
+      </c>
+      <c r="D57" s="26">
+        <f t="shared" si="6"/>
+        <v>645</v>
+      </c>
+      <c r="E57" s="26">
+        <f t="shared" si="7"/>
+        <v>195</v>
+      </c>
+      <c r="F57" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G57" s="51">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H57" s="52">
+        <v>0</v>
+      </c>
+      <c r="I57" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="J57" s="68"/>
+      <c r="L57" s="44"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58" s="26">
+        <v>746</v>
+      </c>
+      <c r="C58" s="26">
+        <v>195</v>
+      </c>
+      <c r="D58" s="26">
+        <f t="shared" si="6"/>
+        <v>746</v>
+      </c>
+      <c r="E58" s="26">
+        <f t="shared" si="7"/>
+        <v>195</v>
+      </c>
+      <c r="F58" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G58" s="51">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H58" s="52">
+        <v>0</v>
+      </c>
+      <c r="I58" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="J58" s="68"/>
+      <c r="L58" s="44"/>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" s="26">
+        <v>847</v>
+      </c>
+      <c r="C59" s="26">
+        <v>195</v>
+      </c>
+      <c r="D59" s="26">
+        <f t="shared" si="6"/>
+        <v>847</v>
+      </c>
+      <c r="E59" s="26">
+        <f t="shared" si="7"/>
+        <v>195</v>
+      </c>
+      <c r="F59" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G59" s="51">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H59" s="52">
+        <v>0</v>
+      </c>
+      <c r="I59" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="J59" s="68"/>
+      <c r="L59" s="44"/>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B52" s="48">
-        <v>150</v>
-      </c>
-      <c r="C52" s="48">
-        <v>193</v>
-      </c>
-      <c r="D52" s="48">
+      <c r="B60" s="26">
+        <v>948</v>
+      </c>
+      <c r="C60" s="26">
+        <v>195</v>
+      </c>
+      <c r="D60" s="26">
         <f t="shared" si="6"/>
-        <v>150</v>
-      </c>
-      <c r="E52" s="48">
+        <v>948</v>
+      </c>
+      <c r="E60" s="26">
         <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="F52" s="31">
+        <v>195</v>
+      </c>
+      <c r="F60" s="26">
         <v>1000</v>
       </c>
-      <c r="G52" s="22">
+      <c r="G60" s="51">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="H52" s="40">
-        <v>0</v>
-      </c>
-      <c r="I52" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="J52" s="63"/>
-      <c r="L52" s="53"/>
-    </row>
-    <row r="53" spans="1:12" ht="15.75">
-      <c r="A53" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="B53" s="48">
-        <v>250</v>
-      </c>
-      <c r="C53" s="48">
-        <v>193</v>
-      </c>
-      <c r="D53" s="48">
+      <c r="H60" s="52">
+        <v>0</v>
+      </c>
+      <c r="I60" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="J60" s="68"/>
+      <c r="L60" s="44"/>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" s="26">
+        <v>1049</v>
+      </c>
+      <c r="C61" s="26">
+        <v>195</v>
+      </c>
+      <c r="D61" s="26">
         <f t="shared" si="6"/>
-        <v>250</v>
-      </c>
-      <c r="E53" s="48">
+        <v>1049</v>
+      </c>
+      <c r="E61" s="26">
         <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="F53" s="31">
+        <v>195</v>
+      </c>
+      <c r="F61" s="26">
         <v>1000</v>
       </c>
-      <c r="G53" s="22">
+      <c r="G61" s="51">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="H53" s="40">
-        <v>0</v>
-      </c>
-      <c r="I53" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="J53" s="63"/>
-      <c r="L53" s="53"/>
-    </row>
-    <row r="54" spans="1:12" ht="15.75">
-      <c r="A54" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="B54" s="48">
-        <v>350</v>
-      </c>
-      <c r="C54" s="48">
-        <v>193</v>
-      </c>
-      <c r="D54" s="48">
-        <f t="shared" si="6"/>
-        <v>350</v>
-      </c>
-      <c r="E54" s="48">
-        <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="F54" s="31">
-        <v>1000</v>
-      </c>
-      <c r="G54" s="22">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="H54" s="40">
-        <v>0</v>
-      </c>
-      <c r="I54" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="J54" s="63"/>
-      <c r="L54" s="53"/>
-    </row>
-    <row r="55" spans="1:12" ht="15.75">
-      <c r="A55" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="B55" s="48">
-        <v>450</v>
-      </c>
-      <c r="C55" s="48">
-        <v>193</v>
-      </c>
-      <c r="D55" s="48">
-        <f t="shared" si="6"/>
-        <v>450</v>
-      </c>
-      <c r="E55" s="48">
-        <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="F55" s="31">
-        <v>1000</v>
-      </c>
-      <c r="G55" s="22">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="H55" s="40">
-        <v>0</v>
-      </c>
-      <c r="I55" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="J55" s="63"/>
-      <c r="L55" s="53"/>
-    </row>
-    <row r="56" spans="1:12" ht="15.75">
-      <c r="A56" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="48">
-        <v>550</v>
-      </c>
-      <c r="C56" s="48">
-        <v>193</v>
-      </c>
-      <c r="D56" s="48">
-        <f t="shared" si="6"/>
-        <v>550</v>
-      </c>
-      <c r="E56" s="48">
-        <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="F56" s="31">
-        <v>1000</v>
-      </c>
-      <c r="G56" s="22">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="H56" s="40">
-        <v>0</v>
-      </c>
-      <c r="I56" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="J56" s="63"/>
-      <c r="L56" s="53"/>
-    </row>
-    <row r="57" spans="1:12" ht="15.75">
-      <c r="A57" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="B57" s="48">
-        <v>650</v>
-      </c>
-      <c r="C57" s="48">
-        <v>193</v>
-      </c>
-      <c r="D57" s="48">
-        <f t="shared" si="6"/>
-        <v>650</v>
-      </c>
-      <c r="E57" s="48">
-        <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="F57" s="31">
-        <v>1000</v>
-      </c>
-      <c r="G57" s="22">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="H57" s="40">
-        <v>0</v>
-      </c>
-      <c r="I57" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="J57" s="63"/>
-      <c r="L57" s="53"/>
-    </row>
-    <row r="58" spans="1:12" ht="15.75">
-      <c r="A58" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="B58" s="48">
-        <v>750</v>
-      </c>
-      <c r="C58" s="48">
-        <v>193</v>
-      </c>
-      <c r="D58" s="48">
-        <f t="shared" si="6"/>
-        <v>750</v>
-      </c>
-      <c r="E58" s="48">
-        <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="F58" s="31">
-        <v>1000</v>
-      </c>
-      <c r="G58" s="22">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="H58" s="40">
-        <v>0</v>
-      </c>
-      <c r="I58" s="49" t="s">
-        <v>92</v>
-      </c>
-      <c r="J58" s="63"/>
-      <c r="L58" s="53"/>
-    </row>
-    <row r="59" spans="1:12" ht="15.75">
-      <c r="A59" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" s="48">
-        <v>850</v>
-      </c>
-      <c r="C59" s="48">
-        <v>193</v>
-      </c>
-      <c r="D59" s="48">
-        <f t="shared" si="6"/>
-        <v>850</v>
-      </c>
-      <c r="E59" s="48">
-        <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="F59" s="31">
-        <v>1000</v>
-      </c>
-      <c r="G59" s="22">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="H59" s="40">
-        <v>0</v>
-      </c>
-      <c r="I59" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="J59" s="63"/>
-      <c r="L59" s="53"/>
-    </row>
-    <row r="60" spans="1:12" ht="15.75">
-      <c r="A60" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="B60" s="48">
-        <v>950</v>
-      </c>
-      <c r="C60" s="48">
-        <v>193</v>
-      </c>
-      <c r="D60" s="48">
-        <f t="shared" si="6"/>
-        <v>950</v>
-      </c>
-      <c r="E60" s="48">
-        <f t="shared" si="7"/>
-        <v>193</v>
-      </c>
-      <c r="F60" s="31">
-        <v>1000</v>
-      </c>
-      <c r="G60" s="22">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="H60" s="40">
-        <v>0</v>
-      </c>
-      <c r="I60" s="49" t="s">
-        <v>132</v>
-      </c>
-      <c r="J60" s="57"/>
-      <c r="L60" s="53"/>
-    </row>
-    <row r="61" spans="1:12" ht="15.75">
-      <c r="A61" s="48" t="s">
+      <c r="H61" s="52">
+        <v>0</v>
+      </c>
+      <c r="I61" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="J61" s="69"/>
+      <c r="L61" s="44"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="B61" s="48">
+      <c r="B62" s="41">
         <v>1770</v>
       </c>
-      <c r="C61" s="48">
+      <c r="C62" s="41">
         <v>60</v>
       </c>
-      <c r="D61" s="48">
+      <c r="D62" s="41">
         <f t="shared" si="6"/>
         <v>1770</v>
       </c>
-      <c r="E61" s="48">
+      <c r="E62" s="41">
         <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="F61" s="31">
+      <c r="F62" s="26">
         <v>2000</v>
       </c>
-      <c r="G61" s="22">
+      <c r="G62" s="19">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="H61" s="40">
-        <v>0</v>
-      </c>
-      <c r="I61" s="49" t="s">
+      <c r="H62" s="35">
+        <v>0</v>
+      </c>
+      <c r="I62" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="J61" s="56" t="s">
+      <c r="J62" s="60" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.75">
-      <c r="A62" s="48" t="s">
+    <row r="63" spans="1:12">
+      <c r="A63" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="B62" s="48">
+      <c r="B63" s="41">
         <v>680</v>
       </c>
-      <c r="C62" s="48">
+      <c r="C63" s="41">
         <v>840</v>
       </c>
-      <c r="D62" s="48">
-        <f t="shared" ref="D62:E67" si="13">B62</f>
+      <c r="D63" s="41">
+        <f t="shared" ref="D63:E68" si="13">B63</f>
         <v>680</v>
       </c>
-      <c r="E62" s="48">
+      <c r="E63" s="41">
         <f t="shared" si="13"/>
         <v>840</v>
       </c>
-      <c r="F62" s="31">
+      <c r="F63" s="26">
         <v>2000</v>
       </c>
-      <c r="G62" s="22">
-        <f t="shared" ref="G62:G67" si="14">F62/1000</f>
+      <c r="G63" s="19">
+        <f t="shared" ref="G63:G68" si="14">F63/1000</f>
         <v>2</v>
       </c>
-      <c r="H62" s="40">
-        <v>0</v>
-      </c>
-      <c r="I62" s="49" t="s">
+      <c r="H63" s="35">
+        <v>0</v>
+      </c>
+      <c r="I63" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="J62" s="57"/>
-    </row>
-    <row r="63" spans="1:12" ht="15.75">
-      <c r="A63" s="48" t="s">
+      <c r="J63" s="61"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="B63" s="48">
+      <c r="B64" s="41">
         <v>1240</v>
       </c>
-      <c r="C63" s="48">
+      <c r="C64" s="41">
         <v>840</v>
       </c>
-      <c r="D63" s="48">
+      <c r="D64" s="41">
         <f t="shared" si="13"/>
         <v>1240</v>
       </c>
-      <c r="E63" s="48">
+      <c r="E64" s="41">
         <f t="shared" si="13"/>
         <v>840</v>
       </c>
-      <c r="F63" s="31">
+      <c r="F64" s="26">
         <v>2000</v>
       </c>
-      <c r="G63" s="22">
+      <c r="G64" s="19">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="H63" s="40">
-        <v>0</v>
-      </c>
-      <c r="I63" s="49" t="s">
+      <c r="H64" s="35">
+        <v>0</v>
+      </c>
+      <c r="I64" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="J63" s="48" t="s">
+      <c r="J64" s="41" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75">
-      <c r="A64" s="48" t="s">
+    <row r="65" spans="1:12">
+      <c r="A65" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="B64" s="48">
+      <c r="B65" s="41">
         <v>250</v>
       </c>
-      <c r="C64" s="48">
+      <c r="C65" s="41">
         <v>1040</v>
       </c>
-      <c r="D64" s="48">
+      <c r="D65" s="41">
         <f t="shared" si="13"/>
         <v>250</v>
       </c>
-      <c r="E64" s="48">
+      <c r="E65" s="41">
         <f t="shared" si="13"/>
         <v>1040</v>
       </c>
-      <c r="F64" s="31">
+      <c r="F65" s="26">
         <v>2000</v>
       </c>
-      <c r="G64" s="22">
+      <c r="G65" s="19">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="H64" s="40">
-        <v>0</v>
-      </c>
-      <c r="I64" s="49" t="s">
+      <c r="H65" s="35">
+        <v>0</v>
+      </c>
+      <c r="I65" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="J64" s="48"/>
-    </row>
-    <row r="65" spans="1:10" ht="15.75">
-      <c r="A65" s="48" t="s">
+      <c r="J65" s="41"/>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="B65" s="48">
+      <c r="B66" s="41">
         <v>670</v>
       </c>
-      <c r="C65" s="48">
+      <c r="C66" s="41">
         <v>475</v>
       </c>
-      <c r="D65" s="48">
+      <c r="D66" s="41">
         <f t="shared" si="13"/>
         <v>670</v>
       </c>
-      <c r="E65" s="48">
+      <c r="E66" s="41">
         <f t="shared" si="13"/>
         <v>475</v>
       </c>
-      <c r="F65" s="31">
+      <c r="F66" s="26">
         <v>2000</v>
       </c>
-      <c r="G65" s="22">
+      <c r="G66" s="19">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="H65" s="40">
-        <v>0</v>
-      </c>
-      <c r="I65" s="49" t="s">
+      <c r="H66" s="35">
+        <v>0</v>
+      </c>
+      <c r="I66" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="J65" s="48"/>
-    </row>
-    <row r="66" spans="1:10" ht="15.75">
-      <c r="A66" s="48" t="s">
+      <c r="J66" s="41"/>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="B66" s="48">
+      <c r="B67" s="41">
         <v>1260</v>
       </c>
-      <c r="C66" s="48">
+      <c r="C67" s="41">
         <v>840</v>
       </c>
-      <c r="D66" s="48">
+      <c r="D67" s="41">
         <f t="shared" si="13"/>
         <v>1260</v>
       </c>
-      <c r="E66" s="48">
+      <c r="E67" s="41">
         <f t="shared" si="13"/>
         <v>840</v>
       </c>
-      <c r="F66" s="31">
+      <c r="F67" s="26">
         <v>2000</v>
       </c>
-      <c r="G66" s="22">
+      <c r="G67" s="19">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="H66" s="40">
-        <v>0</v>
-      </c>
-      <c r="I66" s="49" t="s">
+      <c r="H67" s="35">
+        <v>0</v>
+      </c>
+      <c r="I67" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="J66" s="48" t="s">
+      <c r="J67" s="41" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15.75">
-      <c r="A67" s="48" t="s">
+    <row r="68" spans="1:12">
+      <c r="A68" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="B67" s="48">
+      <c r="B68" s="41">
         <v>660</v>
       </c>
-      <c r="C67" s="48">
+      <c r="C68" s="41">
         <v>840</v>
       </c>
-      <c r="D67" s="48">
+      <c r="D68" s="41">
         <f t="shared" si="13"/>
         <v>660</v>
       </c>
-      <c r="E67" s="48">
+      <c r="E68" s="41">
         <f t="shared" si="13"/>
         <v>840</v>
       </c>
-      <c r="F67" s="31">
+      <c r="F68" s="26">
         <v>2000</v>
       </c>
-      <c r="G67" s="22">
+      <c r="G68" s="19">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="H67" s="40">
-        <v>0</v>
-      </c>
-      <c r="I67" s="49" t="s">
+      <c r="H68" s="35">
+        <v>0</v>
+      </c>
+      <c r="I68" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="J67" s="48"/>
+      <c r="J68" s="41"/>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="47">
+        <v>1500</v>
+      </c>
+      <c r="C69" s="47">
+        <v>100</v>
+      </c>
+      <c r="D69" s="47">
+        <f t="shared" ref="D69" si="15">B69</f>
+        <v>1500</v>
+      </c>
+      <c r="E69" s="47">
+        <f t="shared" ref="E69" si="16">C69</f>
+        <v>100</v>
+      </c>
+      <c r="F69" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G69" s="19">
+        <f t="shared" ref="G69" si="17">F69/1000</f>
+        <v>1</v>
+      </c>
+      <c r="H69" s="35">
+        <v>0</v>
+      </c>
+      <c r="I69" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="J69" s="47"/>
+      <c r="L69" s="44"/>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="48">
+        <v>40</v>
+      </c>
+      <c r="C70" s="48">
+        <v>1015</v>
+      </c>
+      <c r="D70" s="48">
+        <f t="shared" ref="D70" si="18">B70</f>
+        <v>40</v>
+      </c>
+      <c r="E70" s="48">
+        <f t="shared" ref="E70" si="19">C70</f>
+        <v>1015</v>
+      </c>
+      <c r="F70" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G70" s="19">
+        <f t="shared" ref="G70" si="20">F70/1000</f>
+        <v>1</v>
+      </c>
+      <c r="H70" s="35">
+        <v>0</v>
+      </c>
+      <c r="I70" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="J70" s="48"/>
+      <c r="L70" s="44"/>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" s="49">
+        <v>650</v>
+      </c>
+      <c r="C71" s="49">
+        <v>350</v>
+      </c>
+      <c r="D71" s="49">
+        <f t="shared" ref="D71" si="21">B71</f>
+        <v>650</v>
+      </c>
+      <c r="E71" s="49">
+        <f t="shared" ref="E71" si="22">C71</f>
+        <v>350</v>
+      </c>
+      <c r="F71" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G71" s="19">
+        <f t="shared" ref="G71" si="23">F71/1000</f>
+        <v>1</v>
+      </c>
+      <c r="H71" s="35">
+        <v>0</v>
+      </c>
+      <c r="I71" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="J71" s="49"/>
+      <c r="L71" s="44"/>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="B72" s="50">
+        <v>210</v>
+      </c>
+      <c r="C72" s="50">
+        <v>380</v>
+      </c>
+      <c r="D72" s="50">
+        <f t="shared" ref="D72" si="24">B72</f>
+        <v>210</v>
+      </c>
+      <c r="E72" s="50">
+        <f t="shared" ref="E72" si="25">C72</f>
+        <v>380</v>
+      </c>
+      <c r="F72" s="26">
+        <v>1000</v>
+      </c>
+      <c r="G72" s="19">
+        <f t="shared" ref="G72" si="26">F72/1000</f>
+        <v>1</v>
+      </c>
+      <c r="H72" s="35">
+        <v>0</v>
+      </c>
+      <c r="I72" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="J72" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="J3:J11"/>
-    <mergeCell ref="J12:J16"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J51:J60"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I3:I11"/>
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="J61:J62"/>
+    <mergeCell ref="J62:J63"/>
     <mergeCell ref="J28:J32"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J45:J47"/>
@@ -3615,6 +3862,18 @@
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="I35:I40"/>
     <mergeCell ref="I28:I32"/>
+    <mergeCell ref="J51:J61"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I3:I11"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J3:J11"/>
+    <mergeCell ref="J12:J16"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3622,14 +3881,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" s="2" t="s">
@@ -3649,14 +3908,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" s="3" t="s">

</xml_diff>

<commit_message>
6th year update for BGO
</commit_message>
<xml_diff>
--- a/psn/FGO.xlsx
+++ b/psn/FGO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongl2/Desktop/personal/GitHub/fgo-auto-run/psn/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongl2/Desktop/personal/fgo-auto-run/psn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CA3110-62FA-B749-970B-A67D2A368671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1E05E1-1346-A84B-AC91-65F64F734E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28600" yWindow="1740" windowWidth="28080" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="500" windowWidth="29800" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pexel LUT" sheetId="1" r:id="rId1"/>
@@ -512,9 +512,6 @@
     <t>ZHIJIE9</t>
   </si>
   <si>
-    <t>选择助战-职介-8-全</t>
-  </si>
-  <si>
     <t>PYPONT</t>
   </si>
   <si>
@@ -624,6 +621,9 @@
   </si>
   <si>
     <t>固定点按位置</t>
+  </si>
+  <si>
+    <t>选择助战-职介-0-全</t>
   </si>
 </sst>
 </file>
@@ -1046,6 +1046,42 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1058,12 +1094,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1076,40 +1106,10 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1527,8 +1527,8 @@
   <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
+      <pane ySplit="2" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
@@ -1545,18 +1545,18 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="56"/>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="91" t="s">
+      <c r="C1" s="86"/>
+      <c r="D1" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91" t="s">
+      <c r="E1" s="87"/>
+      <c r="F1" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="91"/>
+      <c r="G1" s="87"/>
       <c r="H1" s="33" t="s">
         <v>63</v>
       </c>
@@ -1639,10 +1639,10 @@
       <c r="H3" s="51">
         <v>1</v>
       </c>
-      <c r="I3" s="92" t="s">
+      <c r="I3" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="92" t="s">
+      <c r="J3" s="76" t="s">
         <v>52</v>
       </c>
       <c r="L3" s="43"/>
@@ -1675,8 +1675,8 @@
       <c r="H4" s="51">
         <v>1</v>
       </c>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
       <c r="L4" s="43"/>
     </row>
     <row r="5" spans="1:16">
@@ -1707,8 +1707,8 @@
       <c r="H5" s="51">
         <v>1</v>
       </c>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
       <c r="L5" s="43"/>
     </row>
     <row r="6" spans="1:16">
@@ -1739,8 +1739,8 @@
       <c r="H6" s="51">
         <v>1</v>
       </c>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
       <c r="L6" s="43"/>
     </row>
     <row r="7" spans="1:16">
@@ -1771,8 +1771,8 @@
       <c r="H7" s="51">
         <v>1</v>
       </c>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
       <c r="L7" s="43"/>
     </row>
     <row r="8" spans="1:16">
@@ -1803,8 +1803,8 @@
       <c r="H8" s="51">
         <v>1</v>
       </c>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
       <c r="L8" s="43"/>
     </row>
     <row r="9" spans="1:16">
@@ -1835,8 +1835,8 @@
       <c r="H9" s="51">
         <v>1</v>
       </c>
-      <c r="I9" s="93"/>
-      <c r="J9" s="93"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
       <c r="L9" s="43"/>
     </row>
     <row r="10" spans="1:16">
@@ -1867,8 +1867,8 @@
       <c r="H10" s="51">
         <v>1</v>
       </c>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
       <c r="L10" s="43"/>
     </row>
     <row r="11" spans="1:16">
@@ -1899,8 +1899,8 @@
       <c r="H11" s="51">
         <v>1</v>
       </c>
-      <c r="I11" s="93"/>
-      <c r="J11" s="93"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77"/>
       <c r="L11" s="43"/>
     </row>
     <row r="12" spans="1:16">
@@ -1931,10 +1931,10 @@
       <c r="H12" s="67">
         <v>0</v>
       </c>
-      <c r="I12" s="94" t="s">
+      <c r="I12" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="94" t="s">
+      <c r="J12" s="78" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1966,8 +1966,8 @@
       <c r="H13" s="67">
         <v>0</v>
       </c>
-      <c r="I13" s="95"/>
-      <c r="J13" s="95"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="68" t="s">
@@ -1997,8 +1997,8 @@
       <c r="H14" s="67">
         <v>0</v>
       </c>
-      <c r="I14" s="95"/>
-      <c r="J14" s="95"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="68" t="s">
@@ -2028,8 +2028,8 @@
       <c r="H15" s="67">
         <v>0</v>
       </c>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="68" t="s">
@@ -2059,8 +2059,8 @@
       <c r="H16" s="67">
         <v>0</v>
       </c>
-      <c r="I16" s="95"/>
-      <c r="J16" s="95"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="71" t="s">
@@ -2090,10 +2090,10 @@
       <c r="H17" s="70">
         <v>0</v>
       </c>
-      <c r="I17" s="96" t="s">
+      <c r="I17" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="96" t="s">
+      <c r="J17" s="80" t="s">
         <v>53</v>
       </c>
       <c r="L17" s="44"/>
@@ -2126,8 +2126,8 @@
       <c r="H18" s="70">
         <v>0</v>
       </c>
-      <c r="I18" s="97"/>
-      <c r="J18" s="97"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
       <c r="L18" s="44"/>
     </row>
     <row r="19" spans="1:12">
@@ -2158,8 +2158,8 @@
       <c r="H19" s="70">
         <v>0</v>
       </c>
-      <c r="I19" s="97"/>
-      <c r="J19" s="97"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
       <c r="L19" s="44"/>
     </row>
     <row r="20" spans="1:12">
@@ -2226,10 +2226,10 @@
       <c r="H21" s="73">
         <v>1</v>
       </c>
-      <c r="I21" s="80" t="s">
+      <c r="I21" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="80" t="s">
+      <c r="J21" s="82" t="s">
         <v>52</v>
       </c>
       <c r="L21" s="44"/>
@@ -2262,8 +2262,8 @@
       <c r="H22" s="73">
         <v>1</v>
       </c>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
+      <c r="I22" s="83"/>
+      <c r="J22" s="83"/>
       <c r="L22" s="44"/>
     </row>
     <row r="23" spans="1:12">
@@ -2294,8 +2294,8 @@
       <c r="H23" s="73">
         <v>1</v>
       </c>
-      <c r="I23" s="81"/>
-      <c r="J23" s="81"/>
+      <c r="I23" s="83"/>
+      <c r="J23" s="83"/>
       <c r="L23" s="44"/>
     </row>
     <row r="24" spans="1:12">
@@ -2326,10 +2326,10 @@
       <c r="H24" s="37">
         <v>0</v>
       </c>
-      <c r="I24" s="86" t="s">
+      <c r="I24" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="J24" s="86" t="s">
+      <c r="J24" s="84" t="s">
         <v>53</v>
       </c>
       <c r="L24" s="44"/>
@@ -2362,8 +2362,8 @@
       <c r="H25" s="37">
         <v>0</v>
       </c>
-      <c r="I25" s="87"/>
-      <c r="J25" s="87"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
       <c r="L25" s="44"/>
     </row>
     <row r="26" spans="1:12">
@@ -2394,8 +2394,8 @@
       <c r="H26" s="37">
         <v>0</v>
       </c>
-      <c r="I26" s="87"/>
-      <c r="J26" s="87"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
       <c r="L26" s="44"/>
     </row>
     <row r="27" spans="1:12">
@@ -2461,10 +2461,10 @@
       <c r="H28" s="38">
         <v>0</v>
       </c>
-      <c r="I28" s="78" t="s">
+      <c r="I28" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="J28" s="78" t="s">
+      <c r="J28" s="90" t="s">
         <v>61</v>
       </c>
       <c r="L28" s="44"/>
@@ -2497,8 +2497,8 @@
       <c r="H29" s="38">
         <v>0</v>
       </c>
-      <c r="I29" s="79"/>
-      <c r="J29" s="79"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="91"/>
       <c r="L29" s="44"/>
     </row>
     <row r="30" spans="1:12">
@@ -2529,8 +2529,8 @@
       <c r="H30" s="38">
         <v>0</v>
       </c>
-      <c r="I30" s="79"/>
-      <c r="J30" s="79"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
       <c r="L30" s="44"/>
     </row>
     <row r="31" spans="1:12">
@@ -2561,8 +2561,8 @@
       <c r="H31" s="38">
         <v>0</v>
       </c>
-      <c r="I31" s="79"/>
-      <c r="J31" s="79"/>
+      <c r="I31" s="91"/>
+      <c r="J31" s="91"/>
       <c r="L31" s="44"/>
     </row>
     <row r="32" spans="1:12">
@@ -2593,8 +2593,8 @@
       <c r="H32" s="38">
         <v>0</v>
       </c>
-      <c r="I32" s="79"/>
-      <c r="J32" s="79"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="91"/>
       <c r="L32" s="44"/>
     </row>
     <row r="33" spans="1:12">
@@ -2697,10 +2697,10 @@
       <c r="H35" s="39">
         <v>0</v>
       </c>
-      <c r="I35" s="84" t="s">
+      <c r="I35" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="J35" s="84" t="s">
+      <c r="J35" s="94" t="s">
         <v>53</v>
       </c>
       <c r="L35" s="44"/>
@@ -2733,8 +2733,8 @@
       <c r="H36" s="39">
         <v>0</v>
       </c>
-      <c r="I36" s="85"/>
-      <c r="J36" s="85"/>
+      <c r="I36" s="95"/>
+      <c r="J36" s="95"/>
       <c r="L36" s="44"/>
     </row>
     <row r="37" spans="1:12">
@@ -2765,8 +2765,8 @@
       <c r="H37" s="39">
         <v>0</v>
       </c>
-      <c r="I37" s="85"/>
-      <c r="J37" s="85"/>
+      <c r="I37" s="95"/>
+      <c r="J37" s="95"/>
       <c r="L37" s="44"/>
     </row>
     <row r="38" spans="1:12">
@@ -2797,8 +2797,8 @@
       <c r="H38" s="39">
         <v>0</v>
       </c>
-      <c r="I38" s="85"/>
-      <c r="J38" s="85"/>
+      <c r="I38" s="95"/>
+      <c r="J38" s="95"/>
       <c r="L38" s="44"/>
     </row>
     <row r="39" spans="1:12">
@@ -2829,8 +2829,8 @@
       <c r="H39" s="39">
         <v>0</v>
       </c>
-      <c r="I39" s="85"/>
-      <c r="J39" s="85"/>
+      <c r="I39" s="95"/>
+      <c r="J39" s="95"/>
       <c r="L39" s="44"/>
     </row>
     <row r="40" spans="1:12">
@@ -2861,8 +2861,8 @@
       <c r="H40" s="39">
         <v>0</v>
       </c>
-      <c r="I40" s="85"/>
-      <c r="J40" s="85"/>
+      <c r="I40" s="95"/>
+      <c r="J40" s="95"/>
       <c r="L40" s="44"/>
     </row>
     <row r="41" spans="1:12">
@@ -3037,7 +3037,7 @@
       <c r="I45" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="J45" s="82" t="s">
+      <c r="J45" s="92" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3072,7 +3072,7 @@
       <c r="I46" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="J46" s="83"/>
+      <c r="J46" s="93"/>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="15" t="s">
@@ -3105,7 +3105,7 @@
       <c r="I47" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="J47" s="77"/>
+      <c r="J47" s="89"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="59" t="s">
@@ -3237,14 +3237,14 @@
       <c r="I51" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="J51" s="76" t="s">
+      <c r="J51" s="88" t="s">
         <v>102</v>
       </c>
       <c r="L51" s="54"/>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B52" s="26">
         <v>140</v>
@@ -3271,9 +3271,9 @@
         <v>0</v>
       </c>
       <c r="I52" s="52" t="s">
-        <v>131</v>
-      </c>
-      <c r="J52" s="88"/>
+        <v>168</v>
+      </c>
+      <c r="J52" s="96"/>
       <c r="L52" s="44"/>
     </row>
     <row r="53" spans="1:12">
@@ -3307,7 +3307,7 @@
       <c r="I53" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="J53" s="88"/>
+      <c r="J53" s="96"/>
       <c r="L53" s="44"/>
     </row>
     <row r="54" spans="1:12">
@@ -3341,7 +3341,7 @@
       <c r="I54" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="J54" s="88"/>
+      <c r="J54" s="96"/>
       <c r="L54" s="44"/>
     </row>
     <row r="55" spans="1:12">
@@ -3375,7 +3375,7 @@
       <c r="I55" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="J55" s="88"/>
+      <c r="J55" s="96"/>
       <c r="L55" s="44"/>
     </row>
     <row r="56" spans="1:12">
@@ -3409,7 +3409,7 @@
       <c r="I56" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="J56" s="88"/>
+      <c r="J56" s="96"/>
       <c r="L56" s="44"/>
     </row>
     <row r="57" spans="1:12">
@@ -3443,7 +3443,7 @@
       <c r="I57" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="J57" s="88"/>
+      <c r="J57" s="96"/>
       <c r="L57" s="44"/>
     </row>
     <row r="58" spans="1:12">
@@ -3477,7 +3477,7 @@
       <c r="I58" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="J58" s="88"/>
+      <c r="J58" s="96"/>
       <c r="L58" s="44"/>
     </row>
     <row r="59" spans="1:12">
@@ -3511,7 +3511,7 @@
       <c r="I59" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="J59" s="88"/>
+      <c r="J59" s="96"/>
       <c r="L59" s="44"/>
     </row>
     <row r="60" spans="1:12">
@@ -3543,9 +3543,9 @@
         <v>0</v>
       </c>
       <c r="I60" s="52" t="s">
-        <v>141</v>
-      </c>
-      <c r="J60" s="88"/>
+        <v>140</v>
+      </c>
+      <c r="J60" s="96"/>
       <c r="L60" s="44"/>
     </row>
     <row r="61" spans="1:12">
@@ -3577,9 +3577,9 @@
         <v>0</v>
       </c>
       <c r="I61" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="J61" s="89"/>
+        <v>141</v>
+      </c>
+      <c r="J61" s="97"/>
       <c r="L61" s="44"/>
     </row>
     <row r="62" spans="1:12">
@@ -3613,7 +3613,7 @@
       <c r="I62" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="J62" s="76" t="s">
+      <c r="J62" s="88" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3648,7 +3648,7 @@
       <c r="I63" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="J63" s="77"/>
+      <c r="J63" s="89"/>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="49" t="s">
@@ -3821,7 +3821,7 @@
     </row>
     <row r="69" spans="1:12" s="53" customFormat="1">
       <c r="A69" s="65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B69" s="65">
         <v>1500</v>
@@ -3848,14 +3848,14 @@
         <v>0</v>
       </c>
       <c r="I69" s="52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J69" s="65"/>
       <c r="L69" s="54"/>
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B70" s="47">
         <v>40</v>
@@ -3882,14 +3882,14 @@
         <v>0</v>
       </c>
       <c r="I70" s="42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J70" s="47"/>
       <c r="L70" s="44"/>
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B71" s="48">
         <v>650</v>
@@ -3916,14 +3916,14 @@
         <v>0</v>
       </c>
       <c r="I71" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J71" s="48"/>
       <c r="L71" s="44"/>
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B72" s="49">
         <v>210</v>
@@ -3950,13 +3950,13 @@
         <v>0</v>
       </c>
       <c r="I72" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J72" s="49"/>
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B73" s="15">
         <v>1465</v>
@@ -3983,13 +3983,13 @@
         <v>0</v>
       </c>
       <c r="I73" s="75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J73" s="15"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B74" s="15">
         <v>1690</v>
@@ -4016,13 +4016,13 @@
         <v>0</v>
       </c>
       <c r="I74" s="75" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J74" s="15"/>
     </row>
     <row r="75" spans="1:12">
       <c r="A75" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B75" s="15">
         <v>1730</v>
@@ -4049,13 +4049,13 @@
         <v>0</v>
       </c>
       <c r="I75" s="75" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J75" s="15"/>
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B76" s="15">
         <v>210</v>
@@ -4082,13 +4082,13 @@
         <v>0</v>
       </c>
       <c r="I76" s="75" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J76" s="15"/>
     </row>
     <row r="77" spans="1:12">
       <c r="A77" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B77" s="15">
         <v>660</v>
@@ -4115,13 +4115,13 @@
         <v>0</v>
       </c>
       <c r="I77" s="75" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J77" s="15"/>
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B78" s="15">
         <v>480</v>
@@ -4148,13 +4148,13 @@
         <v>0</v>
       </c>
       <c r="I78" s="75" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J78" s="15"/>
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B79" s="15">
         <v>800</v>
@@ -4181,13 +4181,13 @@
         <v>0</v>
       </c>
       <c r="I79" s="75" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J79" s="15"/>
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B80" s="15">
         <v>1120</v>
@@ -4214,13 +4214,13 @@
         <v>0</v>
       </c>
       <c r="I80" s="75" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J80" s="15"/>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B81" s="15">
         <v>1255</v>
@@ -4247,13 +4247,13 @@
         <v>0</v>
       </c>
       <c r="I81" s="75" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J81" s="15"/>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B82" s="15">
         <v>1650</v>
@@ -4280,13 +4280,13 @@
         <v>0</v>
       </c>
       <c r="I82" s="75" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J82" s="15"/>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B83" s="49">
         <v>1120</v>
@@ -4313,13 +4313,13 @@
         <v>0</v>
       </c>
       <c r="I83" s="42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J83" s="49"/>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B84" s="49">
         <v>1675</v>
@@ -4346,13 +4346,13 @@
         <v>0</v>
       </c>
       <c r="I84" s="42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J84" s="49"/>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B85" s="49">
         <v>627</v>
@@ -4379,23 +4379,12 @@
         <v>0</v>
       </c>
       <c r="I85" s="42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J85" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="J3:J11"/>
-    <mergeCell ref="J12:J16"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="I3:I11"/>
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="F1:G1"/>
     <mergeCell ref="J62:J63"/>
     <mergeCell ref="J28:J32"/>
     <mergeCell ref="I21:I23"/>
@@ -4405,6 +4394,17 @@
     <mergeCell ref="I35:I40"/>
     <mergeCell ref="I28:I32"/>
     <mergeCell ref="J51:J61"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I3:I11"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J3:J11"/>
+    <mergeCell ref="J12:J16"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>